<commit_message>
adding new info to latency and corrected root sampling megapit to NA for KONA and PUUM
</commit_message>
<xml_diff>
--- a/Latency.xlsx
+++ b/Latency.xlsx
@@ -5,23 +5,26 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/clunch/sandbox/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kthibault/Documents/GitHub/sandbox/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{9B820A45-E6A1-2E43-8A36-AC5B68CF8E9A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AA4CB8F3-4FC0-F64B-8658-DE06F1A7BC25}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33340" yWindow="6860" windowWidth="33280" windowHeight="20580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="980" yWindow="460" windowWidth="35600" windowHeight="18840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Wait Times" sheetId="1" r:id="rId1"/>
     <sheet name="Legend" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Wait Times'!$A$1:$I$260</definedName>
+  </definedNames>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1731" uniqueCount="448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1849" uniqueCount="463">
   <si>
     <t>Team</t>
   </si>
@@ -1365,13 +1368,58 @@
   </si>
   <si>
     <t>Field data only; latency allows time for field ecologists to collect all data in a bout and QA data</t>
+  </si>
+  <si>
+    <t>Legacy ingest status (%)</t>
+  </si>
+  <si>
+    <t>Legacy delay driver</t>
+  </si>
+  <si>
+    <t>contracting</t>
+  </si>
+  <si>
+    <t>external lab processing</t>
+  </si>
+  <si>
+    <t>Vendor identified; contracting process prolonged</t>
+  </si>
+  <si>
+    <t>science resources</t>
+  </si>
+  <si>
+    <t>Waiting on HQ Scientist availability to ingest final error corrected records</t>
+  </si>
+  <si>
+    <t>U WY lab not returning data on time; samples backlogged</t>
+  </si>
+  <si>
+    <t>Expected Legacy Ingest Completion</t>
+  </si>
+  <si>
+    <t>field science resources</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waiting for field staff to conduct protocol again  to resolve errors </t>
+  </si>
+  <si>
+    <t>Legacy Data notes</t>
+  </si>
+  <si>
+    <t>Waiting on HQ Scientist availability to correct sampleID errors that allow for data ingest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Waiting for field staff to conduct protocol again to efficiently resolve errors </t>
+  </si>
+  <si>
+    <t>Waiting on HQ Scientist availability to conduct QA and upload 2017 data</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1502,6 +1550,13 @@
     <font>
       <sz val="12"/>
       <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1848,8 +1903,13 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2205,24 +2265,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:I260"/>
+  <dimension ref="A1:M260"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="G44" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomRight" activeCell="J61" sqref="J61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="28" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="71" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="40.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="41.33203125" customWidth="1"/>
+    <col min="4" max="4" width="33.5" customWidth="1"/>
     <col min="6" max="6" width="16.5" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="18" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="4" customWidth="1"/>
     <col min="9" max="9" width="14.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" ht="64" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2247,8 +2310,20 @@
       <c r="I1" t="s">
         <v>432</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J1" s="1" t="s">
+        <v>448</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>449</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>456</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -2273,8 +2348,17 @@
       <c r="I2" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J2">
+        <v>100</v>
+      </c>
+      <c r="K2" t="s">
+        <v>7</v>
+      </c>
+      <c r="L2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -2299,8 +2383,17 @@
       <c r="I3" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J3">
+        <v>100</v>
+      </c>
+      <c r="K3" t="s">
+        <v>7</v>
+      </c>
+      <c r="L3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -2325,8 +2418,17 @@
       <c r="I4" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J4">
+        <v>100</v>
+      </c>
+      <c r="K4" t="s">
+        <v>7</v>
+      </c>
+      <c r="L4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -2351,8 +2453,17 @@
       <c r="I5" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J5">
+        <v>100</v>
+      </c>
+      <c r="K5" t="s">
+        <v>7</v>
+      </c>
+      <c r="L5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>2</v>
       </c>
@@ -2377,8 +2488,17 @@
       <c r="I6" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J6" t="s">
+        <v>7</v>
+      </c>
+      <c r="K6" t="s">
+        <v>7</v>
+      </c>
+      <c r="L6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -2403,8 +2523,17 @@
       <c r="I7" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J7">
+        <v>90</v>
+      </c>
+      <c r="K7" t="s">
+        <v>7</v>
+      </c>
+      <c r="L7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
@@ -2429,8 +2558,17 @@
       <c r="I8" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J8">
+        <v>90</v>
+      </c>
+      <c r="K8" t="s">
+        <v>7</v>
+      </c>
+      <c r="L8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>2</v>
       </c>
@@ -2455,8 +2593,17 @@
       <c r="I9" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J9">
+        <v>90</v>
+      </c>
+      <c r="K9" t="s">
+        <v>7</v>
+      </c>
+      <c r="L9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>2</v>
       </c>
@@ -2481,8 +2628,17 @@
       <c r="I10" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J10">
+        <v>100</v>
+      </c>
+      <c r="K10" t="s">
+        <v>7</v>
+      </c>
+      <c r="L10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>2</v>
       </c>
@@ -2507,8 +2663,17 @@
       <c r="I11" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J11">
+        <v>100</v>
+      </c>
+      <c r="K11" t="s">
+        <v>7</v>
+      </c>
+      <c r="L11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>2</v>
       </c>
@@ -2533,8 +2698,20 @@
       <c r="I12" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J12">
+        <v>12</v>
+      </c>
+      <c r="K12" t="s">
+        <v>450</v>
+      </c>
+      <c r="L12" s="2">
+        <v>43374</v>
+      </c>
+      <c r="M12" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>2</v>
       </c>
@@ -2559,8 +2736,20 @@
       <c r="I13" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J13">
+        <v>12</v>
+      </c>
+      <c r="K13" t="s">
+        <v>450</v>
+      </c>
+      <c r="L13" s="2">
+        <v>43374</v>
+      </c>
+      <c r="M13" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>2</v>
       </c>
@@ -2585,8 +2774,20 @@
       <c r="I14" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J14">
+        <v>12</v>
+      </c>
+      <c r="K14" t="s">
+        <v>450</v>
+      </c>
+      <c r="L14" s="2">
+        <v>43374</v>
+      </c>
+      <c r="M14" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>2</v>
       </c>
@@ -2611,8 +2812,20 @@
       <c r="I15" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J15">
+        <v>12</v>
+      </c>
+      <c r="K15" t="s">
+        <v>450</v>
+      </c>
+      <c r="L15" s="2">
+        <v>43374</v>
+      </c>
+      <c r="M15" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>2</v>
       </c>
@@ -2637,8 +2850,17 @@
       <c r="I16" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J16">
+        <v>100</v>
+      </c>
+      <c r="K16" t="s">
+        <v>7</v>
+      </c>
+      <c r="L16" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>2</v>
       </c>
@@ -2663,8 +2885,20 @@
       <c r="I17" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J17">
+        <v>80</v>
+      </c>
+      <c r="K17" t="s">
+        <v>450</v>
+      </c>
+      <c r="L17" s="2">
+        <v>43374</v>
+      </c>
+      <c r="M17" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>2</v>
       </c>
@@ -2689,8 +2923,20 @@
       <c r="I18" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J18">
+        <v>80</v>
+      </c>
+      <c r="K18" t="s">
+        <v>450</v>
+      </c>
+      <c r="L18" s="2">
+        <v>43374</v>
+      </c>
+      <c r="M18" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -2715,8 +2961,17 @@
       <c r="I19" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J19">
+        <v>100</v>
+      </c>
+      <c r="K19" t="s">
+        <v>7</v>
+      </c>
+      <c r="L19" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>2</v>
       </c>
@@ -2741,8 +2996,17 @@
       <c r="I20" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J20">
+        <v>100</v>
+      </c>
+      <c r="K20" t="s">
+        <v>7</v>
+      </c>
+      <c r="L20" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>2</v>
       </c>
@@ -2767,8 +3031,17 @@
       <c r="I21" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J21">
+        <v>100</v>
+      </c>
+      <c r="K21" t="s">
+        <v>7</v>
+      </c>
+      <c r="L21" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>2</v>
       </c>
@@ -2793,8 +3066,20 @@
       <c r="I22" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J22">
+        <v>95</v>
+      </c>
+      <c r="K22" t="s">
+        <v>453</v>
+      </c>
+      <c r="L22" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M22" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>2</v>
       </c>
@@ -2819,8 +3104,20 @@
       <c r="I23" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J23">
+        <v>95</v>
+      </c>
+      <c r="K23" t="s">
+        <v>453</v>
+      </c>
+      <c r="L23" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M23" t="s">
+        <v>454</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>2</v>
       </c>
@@ -2845,8 +3142,20 @@
       <c r="I24" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J24">
+        <v>60</v>
+      </c>
+      <c r="K24" t="s">
+        <v>451</v>
+      </c>
+      <c r="L24" s="2">
+        <v>43344</v>
+      </c>
+      <c r="M24" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>2</v>
       </c>
@@ -2871,8 +3180,17 @@
       <c r="I25" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J25">
+        <v>100</v>
+      </c>
+      <c r="K25" t="s">
+        <v>7</v>
+      </c>
+      <c r="L25" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>2</v>
       </c>
@@ -2897,8 +3215,20 @@
       <c r="I26" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J26">
+        <v>30</v>
+      </c>
+      <c r="K26" t="s">
+        <v>451</v>
+      </c>
+      <c r="L26" s="2">
+        <v>43344</v>
+      </c>
+      <c r="M26" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>2</v>
       </c>
@@ -2923,8 +3253,17 @@
       <c r="I27" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J27">
+        <v>100</v>
+      </c>
+      <c r="K27" t="s">
+        <v>7</v>
+      </c>
+      <c r="L27" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>2</v>
       </c>
@@ -2949,8 +3288,17 @@
       <c r="I28" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J28">
+        <v>100</v>
+      </c>
+      <c r="K28" t="s">
+        <v>7</v>
+      </c>
+      <c r="L28" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>2</v>
       </c>
@@ -2975,8 +3323,17 @@
       <c r="I29" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J29">
+        <v>100</v>
+      </c>
+      <c r="K29" t="s">
+        <v>7</v>
+      </c>
+      <c r="L29" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>2</v>
       </c>
@@ -3001,8 +3358,17 @@
       <c r="I30" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J30">
+        <v>100</v>
+      </c>
+      <c r="K30" t="s">
+        <v>7</v>
+      </c>
+      <c r="L30" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>2</v>
       </c>
@@ -3027,8 +3393,20 @@
       <c r="I31" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J31">
+        <v>7</v>
+      </c>
+      <c r="K31" t="s">
+        <v>450</v>
+      </c>
+      <c r="L31" s="2">
+        <v>43374</v>
+      </c>
+      <c r="M31" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>2</v>
       </c>
@@ -3053,8 +3431,20 @@
       <c r="I32" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J32">
+        <v>7</v>
+      </c>
+      <c r="K32" t="s">
+        <v>450</v>
+      </c>
+      <c r="L32" s="2">
+        <v>43374</v>
+      </c>
+      <c r="M32" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>2</v>
       </c>
@@ -3079,8 +3469,20 @@
       <c r="I33" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J33">
+        <v>7</v>
+      </c>
+      <c r="K33" t="s">
+        <v>450</v>
+      </c>
+      <c r="L33" s="2">
+        <v>43374</v>
+      </c>
+      <c r="M33" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>2</v>
       </c>
@@ -3105,8 +3507,20 @@
       <c r="I34" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J34">
+        <v>7</v>
+      </c>
+      <c r="K34" t="s">
+        <v>450</v>
+      </c>
+      <c r="L34" s="2">
+        <v>43374</v>
+      </c>
+      <c r="M34" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>2</v>
       </c>
@@ -3131,8 +3545,20 @@
       <c r="I35" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J35">
+        <v>6</v>
+      </c>
+      <c r="K35" t="s">
+        <v>450</v>
+      </c>
+      <c r="L35" s="2">
+        <v>43435</v>
+      </c>
+      <c r="M35" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>2</v>
       </c>
@@ -3157,8 +3583,20 @@
       <c r="I36" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J36">
+        <v>6</v>
+      </c>
+      <c r="K36" t="s">
+        <v>450</v>
+      </c>
+      <c r="L36" s="2">
+        <v>43435</v>
+      </c>
+      <c r="M36" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>2</v>
       </c>
@@ -3183,8 +3621,20 @@
       <c r="I37" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J37">
+        <v>70</v>
+      </c>
+      <c r="K37" t="s">
+        <v>453</v>
+      </c>
+      <c r="L37" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M37" s="3" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>2</v>
       </c>
@@ -3209,8 +3659,20 @@
       <c r="I38" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J38">
+        <v>7</v>
+      </c>
+      <c r="K38" t="s">
+        <v>450</v>
+      </c>
+      <c r="L38" s="2">
+        <v>43435</v>
+      </c>
+      <c r="M38" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>2</v>
       </c>
@@ -3235,8 +3697,20 @@
       <c r="I39" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J39">
+        <v>70</v>
+      </c>
+      <c r="K39" t="s">
+        <v>453</v>
+      </c>
+      <c r="L39" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M39" s="3" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>2</v>
       </c>
@@ -3261,8 +3735,20 @@
       <c r="I40" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J40">
+        <v>70</v>
+      </c>
+      <c r="K40" t="s">
+        <v>453</v>
+      </c>
+      <c r="L40" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M40" s="3" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>2</v>
       </c>
@@ -3287,8 +3773,14 @@
       <c r="I41" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J41">
+        <v>100</v>
+      </c>
+      <c r="K41" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>2</v>
       </c>
@@ -3313,8 +3805,14 @@
       <c r="I42" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J42">
+        <v>100</v>
+      </c>
+      <c r="K42" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>2</v>
       </c>
@@ -3339,8 +3837,20 @@
       <c r="I43" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J43">
+        <v>90</v>
+      </c>
+      <c r="K43" t="s">
+        <v>457</v>
+      </c>
+      <c r="L43" s="2">
+        <v>43435</v>
+      </c>
+      <c r="M43" t="s">
+        <v>461</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>2</v>
       </c>
@@ -3365,8 +3875,14 @@
       <c r="I44" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J44">
+        <v>100</v>
+      </c>
+      <c r="K44" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>2</v>
       </c>
@@ -3391,8 +3907,14 @@
       <c r="I45" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J45">
+        <v>100</v>
+      </c>
+      <c r="K45" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>2</v>
       </c>
@@ -3417,8 +3939,14 @@
       <c r="I46" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J46">
+        <v>100</v>
+      </c>
+      <c r="K46" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>2</v>
       </c>
@@ -3443,8 +3971,14 @@
       <c r="I47" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J47">
+        <v>100</v>
+      </c>
+      <c r="K47" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>2</v>
       </c>
@@ -3469,8 +4003,14 @@
       <c r="I48" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J48">
+        <v>100</v>
+      </c>
+      <c r="K48" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>2</v>
       </c>
@@ -3495,8 +4035,14 @@
       <c r="I49" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J49">
+        <v>100</v>
+      </c>
+      <c r="K49" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>2</v>
       </c>
@@ -3521,8 +4067,14 @@
       <c r="I50" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J50">
+        <v>100</v>
+      </c>
+      <c r="K50" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>2</v>
       </c>
@@ -3547,8 +4099,20 @@
       <c r="I51" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J51">
+        <v>75</v>
+      </c>
+      <c r="K51" t="s">
+        <v>451</v>
+      </c>
+      <c r="L51" s="2">
+        <v>43344</v>
+      </c>
+      <c r="M51" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>2</v>
       </c>
@@ -3573,8 +4137,14 @@
       <c r="I52" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J52">
+        <v>100</v>
+      </c>
+      <c r="K52" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>2</v>
       </c>
@@ -3599,8 +4169,14 @@
       <c r="I53" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J53">
+        <v>100</v>
+      </c>
+      <c r="K53" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>2</v>
       </c>
@@ -3625,8 +4201,14 @@
       <c r="I54" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J54">
+        <v>100</v>
+      </c>
+      <c r="K54" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>2</v>
       </c>
@@ -3651,8 +4233,14 @@
       <c r="I55" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J55">
+        <v>100</v>
+      </c>
+      <c r="K55" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>2</v>
       </c>
@@ -3677,8 +4265,14 @@
       <c r="I56" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J56">
+        <v>100</v>
+      </c>
+      <c r="K56" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>2</v>
       </c>
@@ -3703,8 +4297,14 @@
       <c r="I57" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J57">
+        <v>100</v>
+      </c>
+      <c r="K57" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>2</v>
       </c>
@@ -3729,8 +4329,14 @@
       <c r="I58" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J58">
+        <v>100</v>
+      </c>
+      <c r="K58" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A59" t="s">
         <v>2</v>
       </c>
@@ -3755,8 +4361,20 @@
       <c r="I59" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J59">
+        <v>60</v>
+      </c>
+      <c r="K59" t="s">
+        <v>453</v>
+      </c>
+      <c r="L59" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M59" t="s">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
         <v>2</v>
       </c>
@@ -3781,8 +4399,20 @@
       <c r="I60" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J60">
+        <v>50</v>
+      </c>
+      <c r="K60" t="s">
+        <v>451</v>
+      </c>
+      <c r="L60" s="2">
+        <v>43344</v>
+      </c>
+      <c r="M60" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
         <v>2</v>
       </c>
@@ -3808,7 +4438,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
         <v>2</v>
       </c>
@@ -3834,7 +4464,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
         <v>2</v>
       </c>
@@ -3860,7 +4490,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
         <v>2</v>
       </c>
@@ -3886,7 +4516,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>2</v>
       </c>
@@ -3912,7 +4542,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>2</v>
       </c>
@@ -3938,7 +4568,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>2</v>
       </c>
@@ -3964,7 +4594,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>2</v>
       </c>
@@ -3990,7 +4620,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>2</v>
       </c>
@@ -4015,8 +4645,14 @@
       <c r="I69" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J69">
+        <v>100</v>
+      </c>
+      <c r="K69" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>2</v>
       </c>
@@ -4041,8 +4677,14 @@
       <c r="I70" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J70">
+        <v>100</v>
+      </c>
+      <c r="K70" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>2</v>
       </c>
@@ -4067,8 +4709,14 @@
       <c r="I71" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J71">
+        <v>100</v>
+      </c>
+      <c r="K71" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>2</v>
       </c>
@@ -4094,7 +4742,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>2</v>
       </c>
@@ -4120,7 +4768,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>2</v>
       </c>
@@ -4146,7 +4794,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>2</v>
       </c>
@@ -4172,7 +4820,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>2</v>
       </c>
@@ -4198,7 +4846,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>2</v>
       </c>
@@ -4224,7 +4872,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>2</v>
       </c>
@@ -4250,7 +4898,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>2</v>
       </c>
@@ -4276,7 +4924,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>2</v>
       </c>
@@ -5134,7 +5782,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
         <v>2</v>
       </c>
@@ -5160,7 +5808,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
         <v>2</v>
       </c>
@@ -5186,7 +5834,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
         <v>2</v>
       </c>
@@ -5212,7 +5860,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
         <v>2</v>
       </c>
@@ -5238,7 +5886,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
         <v>2</v>
       </c>
@@ -5263,8 +5911,20 @@
       <c r="I117" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J117">
+        <v>90</v>
+      </c>
+      <c r="K117" t="s">
+        <v>457</v>
+      </c>
+      <c r="L117" s="2">
+        <v>43435</v>
+      </c>
+      <c r="M117" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A118" t="s">
         <v>2</v>
       </c>
@@ -5289,8 +5949,20 @@
       <c r="I118" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J118">
+        <v>90</v>
+      </c>
+      <c r="K118" t="s">
+        <v>457</v>
+      </c>
+      <c r="L118" s="2">
+        <v>43435</v>
+      </c>
+      <c r="M118" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A119" t="s">
         <v>2</v>
       </c>
@@ -5315,8 +5987,20 @@
       <c r="I119" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J119">
+        <v>90</v>
+      </c>
+      <c r="K119" t="s">
+        <v>457</v>
+      </c>
+      <c r="L119" s="2">
+        <v>43435</v>
+      </c>
+      <c r="M119" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A120" t="s">
         <v>2</v>
       </c>
@@ -5341,8 +6025,20 @@
       <c r="I120" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J120">
+        <v>90</v>
+      </c>
+      <c r="K120" t="s">
+        <v>457</v>
+      </c>
+      <c r="L120" s="2">
+        <v>43435</v>
+      </c>
+      <c r="M120" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="121" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A121" t="s">
         <v>209</v>
       </c>
@@ -5368,7 +6064,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
         <v>209</v>
       </c>
@@ -5394,7 +6090,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
         <v>209</v>
       </c>
@@ -5420,7 +6116,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
         <v>209</v>
       </c>
@@ -5446,7 +6142,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
         <v>209</v>
       </c>
@@ -5472,7 +6168,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
         <v>209</v>
       </c>
@@ -5498,7 +6194,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
         <v>209</v>
       </c>
@@ -5524,7 +6220,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
         <v>209</v>
       </c>
@@ -8983,6 +9679,7 @@
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:I260" xr:uid="{F920CE2C-728A-1C45-9F6A-0B2E6D995C2C}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -8992,7 +9689,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added more latency info for TOS dps
</commit_message>
<xml_diff>
--- a/Latency.xlsx
+++ b/Latency.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kthibault/Documents/GitHub/sandbox/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{AA4CB8F3-4FC0-F64B-8658-DE06F1A7BC25}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D7CA9A5C-3DBF-3C49-AAFC-D2D0F4FAD86E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="980" yWindow="460" windowWidth="35600" windowHeight="18840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="760" yWindow="1680" windowWidth="35600" windowHeight="18840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Wait Times" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1849" uniqueCount="463">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1940" uniqueCount="469">
   <si>
     <t>Team</t>
   </si>
@@ -1413,6 +1413,24 @@
   </si>
   <si>
     <t>Waiting on HQ Scientist availability to conduct QA and upload 2017 data</t>
+  </si>
+  <si>
+    <t>MBL lab not returning data on time; samples backlogged</t>
+  </si>
+  <si>
+    <t>MBL lab not returning soil data on time; samples backlogged; dependency</t>
+  </si>
+  <si>
+    <t>NRCS not returning data on time; samples backlogged</t>
+  </si>
+  <si>
+    <t>NRCS not returning data on time</t>
+  </si>
+  <si>
+    <t>Waiting on HQ Scientist availability to complete error correction of 2013 data</t>
+  </si>
+  <si>
+    <t>Awaiting 2017 data - proceeding on schedule; requires final sampling bout for year to be completed; all ticks identified to species; then samples selected for pathogen testing</t>
   </si>
 </sst>
 </file>
@@ -1562,7 +1580,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1742,6 +1760,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1903,13 +1927,14 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2268,10 +2293,10 @@
   <dimension ref="A1:M260"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="G44" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="G12" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J61" sqref="J61"/>
+      <selection pane="bottomRight" activeCell="O18" sqref="O18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4437,6 +4462,18 @@
       <c r="I61" t="s">
         <v>441</v>
       </c>
+      <c r="J61">
+        <v>80</v>
+      </c>
+      <c r="K61" t="s">
+        <v>451</v>
+      </c>
+      <c r="L61" s="2">
+        <v>43344</v>
+      </c>
+      <c r="M61" t="s">
+        <v>464</v>
+      </c>
     </row>
     <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
@@ -4463,6 +4500,18 @@
       <c r="I62" t="s">
         <v>441</v>
       </c>
+      <c r="J62">
+        <v>80</v>
+      </c>
+      <c r="K62" t="s">
+        <v>451</v>
+      </c>
+      <c r="L62" s="2">
+        <v>43344</v>
+      </c>
+      <c r="M62" t="s">
+        <v>464</v>
+      </c>
     </row>
     <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
@@ -4489,6 +4538,18 @@
       <c r="I63" t="s">
         <v>441</v>
       </c>
+      <c r="J63">
+        <v>80</v>
+      </c>
+      <c r="K63" t="s">
+        <v>451</v>
+      </c>
+      <c r="L63" s="2">
+        <v>43344</v>
+      </c>
+      <c r="M63" t="s">
+        <v>464</v>
+      </c>
     </row>
     <row r="64" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
@@ -4515,8 +4576,17 @@
       <c r="I64" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J64">
+        <v>100</v>
+      </c>
+      <c r="K64" t="s">
+        <v>7</v>
+      </c>
+      <c r="L64" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>2</v>
       </c>
@@ -4541,8 +4611,17 @@
       <c r="I65" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J65">
+        <v>100</v>
+      </c>
+      <c r="K65" t="s">
+        <v>7</v>
+      </c>
+      <c r="L65" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>2</v>
       </c>
@@ -4567,8 +4646,17 @@
       <c r="I66" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J66">
+        <v>100</v>
+      </c>
+      <c r="K66" t="s">
+        <v>7</v>
+      </c>
+      <c r="L66" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>2</v>
       </c>
@@ -4593,8 +4681,17 @@
       <c r="I67" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J67">
+        <v>100</v>
+      </c>
+      <c r="K67" t="s">
+        <v>7</v>
+      </c>
+      <c r="L67" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>2</v>
       </c>
@@ -4619,8 +4716,20 @@
       <c r="I68" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J68">
+        <v>50</v>
+      </c>
+      <c r="K68" t="s">
+        <v>451</v>
+      </c>
+      <c r="L68" s="2">
+        <v>43344</v>
+      </c>
+      <c r="M68" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>2</v>
       </c>
@@ -4652,7 +4761,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>2</v>
       </c>
@@ -4684,7 +4793,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>2</v>
       </c>
@@ -4716,7 +4825,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>2</v>
       </c>
@@ -4741,8 +4850,20 @@
       <c r="I72" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J72">
+        <v>6</v>
+      </c>
+      <c r="K72" t="s">
+        <v>450</v>
+      </c>
+      <c r="L72" s="2">
+        <v>43374</v>
+      </c>
+      <c r="M72" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>2</v>
       </c>
@@ -4767,8 +4888,20 @@
       <c r="I73" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J73">
+        <v>6</v>
+      </c>
+      <c r="K73" t="s">
+        <v>450</v>
+      </c>
+      <c r="L73" s="2">
+        <v>43374</v>
+      </c>
+      <c r="M73" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>2</v>
       </c>
@@ -4793,8 +4926,20 @@
       <c r="I74" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J74">
+        <v>6</v>
+      </c>
+      <c r="K74" t="s">
+        <v>450</v>
+      </c>
+      <c r="L74" s="2">
+        <v>43374</v>
+      </c>
+      <c r="M74" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>2</v>
       </c>
@@ -4819,8 +4964,20 @@
       <c r="I75" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J75">
+        <v>6</v>
+      </c>
+      <c r="K75" t="s">
+        <v>450</v>
+      </c>
+      <c r="L75" s="2">
+        <v>43374</v>
+      </c>
+      <c r="M75" t="s">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>2</v>
       </c>
@@ -4845,8 +5002,20 @@
       <c r="I76" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J76">
+        <v>15</v>
+      </c>
+      <c r="K76" t="s">
+        <v>451</v>
+      </c>
+      <c r="L76" s="2">
+        <v>43465</v>
+      </c>
+      <c r="M76" t="s">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>2</v>
       </c>
@@ -4871,8 +5040,20 @@
       <c r="I77" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J77">
+        <v>95</v>
+      </c>
+      <c r="K77" t="s">
+        <v>451</v>
+      </c>
+      <c r="L77" s="2">
+        <v>43344</v>
+      </c>
+      <c r="M77" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>2</v>
       </c>
@@ -4897,8 +5078,20 @@
       <c r="I78" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J78">
+        <v>75</v>
+      </c>
+      <c r="K78" t="s">
+        <v>451</v>
+      </c>
+      <c r="L78" s="2">
+        <v>43344</v>
+      </c>
+      <c r="M78" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>2</v>
       </c>
@@ -4923,8 +5116,20 @@
       <c r="I79" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="J79">
+        <v>75</v>
+      </c>
+      <c r="K79" t="s">
+        <v>451</v>
+      </c>
+      <c r="L79" s="2">
+        <v>43344</v>
+      </c>
+      <c r="M79" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>2</v>
       </c>
@@ -4949,8 +5154,20 @@
       <c r="I80" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J80">
+        <v>75</v>
+      </c>
+      <c r="K80" t="s">
+        <v>451</v>
+      </c>
+      <c r="L80" s="2">
+        <v>43344</v>
+      </c>
+      <c r="M80" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
         <v>2</v>
       </c>
@@ -4975,8 +5192,20 @@
       <c r="I81" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J81">
+        <v>75</v>
+      </c>
+      <c r="K81" t="s">
+        <v>451</v>
+      </c>
+      <c r="L81" s="2">
+        <v>43344</v>
+      </c>
+      <c r="M81" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
         <v>2</v>
       </c>
@@ -5001,8 +5230,16 @@
       <c r="I82" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J82">
+        <v>70</v>
+      </c>
+      <c r="K82" t="s">
+        <v>451</v>
+      </c>
+      <c r="L82" s="4"/>
+      <c r="M82" s="4"/>
+    </row>
+    <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
         <v>2</v>
       </c>
@@ -5027,8 +5264,16 @@
       <c r="I83" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J83">
+        <v>70</v>
+      </c>
+      <c r="K83" t="s">
+        <v>451</v>
+      </c>
+      <c r="L83" s="4"/>
+      <c r="M83" s="4"/>
+    </row>
+    <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
         <v>2</v>
       </c>
@@ -5053,8 +5298,16 @@
       <c r="I84" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J84">
+        <v>70</v>
+      </c>
+      <c r="K84" t="s">
+        <v>451</v>
+      </c>
+      <c r="L84" s="4"/>
+      <c r="M84" s="4"/>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
         <v>2</v>
       </c>
@@ -5079,8 +5332,16 @@
       <c r="I85" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J85">
+        <v>1</v>
+      </c>
+      <c r="K85" t="s">
+        <v>451</v>
+      </c>
+      <c r="L85" s="4"/>
+      <c r="M85" s="4"/>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
         <v>2</v>
       </c>
@@ -5105,8 +5366,16 @@
       <c r="I86" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J86">
+        <v>1</v>
+      </c>
+      <c r="K86" t="s">
+        <v>451</v>
+      </c>
+      <c r="L86" s="4"/>
+      <c r="M86" s="4"/>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
         <v>2</v>
       </c>
@@ -5131,8 +5400,16 @@
       <c r="I87" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J87">
+        <v>2</v>
+      </c>
+      <c r="K87" t="s">
+        <v>451</v>
+      </c>
+      <c r="L87" s="4"/>
+      <c r="M87" s="4"/>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
         <v>2</v>
       </c>
@@ -5157,8 +5434,16 @@
       <c r="I88" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J88">
+        <v>5</v>
+      </c>
+      <c r="K88" t="s">
+        <v>451</v>
+      </c>
+      <c r="L88" s="4"/>
+      <c r="M88" s="4"/>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
         <v>2</v>
       </c>
@@ -5183,8 +5468,16 @@
       <c r="I89" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J89">
+        <v>5</v>
+      </c>
+      <c r="K89" t="s">
+        <v>451</v>
+      </c>
+      <c r="L89" s="4"/>
+      <c r="M89" s="4"/>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>2</v>
       </c>
@@ -5209,8 +5502,16 @@
       <c r="I90" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J90">
+        <v>6</v>
+      </c>
+      <c r="K90" t="s">
+        <v>451</v>
+      </c>
+      <c r="L90" s="4"/>
+      <c r="M90" s="4"/>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
         <v>2</v>
       </c>
@@ -5235,8 +5536,16 @@
       <c r="I91" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J91">
+        <v>6</v>
+      </c>
+      <c r="K91" t="s">
+        <v>451</v>
+      </c>
+      <c r="L91" s="4"/>
+      <c r="M91" s="4"/>
+    </row>
+    <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>2</v>
       </c>
@@ -5261,8 +5570,16 @@
       <c r="I92" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J92">
+        <v>6</v>
+      </c>
+      <c r="K92" t="s">
+        <v>451</v>
+      </c>
+      <c r="L92" s="4"/>
+      <c r="M92" s="4"/>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>2</v>
       </c>
@@ -5287,8 +5604,16 @@
       <c r="I93" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J93">
+        <v>6</v>
+      </c>
+      <c r="K93" t="s">
+        <v>451</v>
+      </c>
+      <c r="L93" s="4"/>
+      <c r="M93" s="4"/>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>2</v>
       </c>
@@ -5313,8 +5638,16 @@
       <c r="I94" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J94">
+        <v>6</v>
+      </c>
+      <c r="K94" t="s">
+        <v>451</v>
+      </c>
+      <c r="L94" s="4"/>
+      <c r="M94" s="4"/>
+    </row>
+    <row r="95" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>2</v>
       </c>
@@ -5339,8 +5672,16 @@
       <c r="I95" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J95">
+        <v>5</v>
+      </c>
+      <c r="K95" t="s">
+        <v>451</v>
+      </c>
+      <c r="L95" s="4"/>
+      <c r="M95" s="4"/>
+    </row>
+    <row r="96" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
         <v>2</v>
       </c>
@@ -5365,8 +5706,16 @@
       <c r="I96" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J96">
+        <v>5</v>
+      </c>
+      <c r="K96" t="s">
+        <v>451</v>
+      </c>
+      <c r="L96" s="4"/>
+      <c r="M96" s="4"/>
+    </row>
+    <row r="97" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
         <v>2</v>
       </c>
@@ -5391,8 +5740,20 @@
       <c r="I97" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J97">
+        <v>15</v>
+      </c>
+      <c r="K97" t="s">
+        <v>451</v>
+      </c>
+      <c r="L97" s="2">
+        <v>43465</v>
+      </c>
+      <c r="M97" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="98" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A98" t="s">
         <v>2</v>
       </c>
@@ -5417,8 +5778,20 @@
       <c r="I98" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J98">
+        <v>15</v>
+      </c>
+      <c r="K98" t="s">
+        <v>451</v>
+      </c>
+      <c r="L98" s="2">
+        <v>43465</v>
+      </c>
+      <c r="M98" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
         <v>2</v>
       </c>
@@ -5443,8 +5816,20 @@
       <c r="I99" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J99">
+        <v>15</v>
+      </c>
+      <c r="K99" t="s">
+        <v>451</v>
+      </c>
+      <c r="L99" s="2">
+        <v>43465</v>
+      </c>
+      <c r="M99" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="100" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A100" t="s">
         <v>2</v>
       </c>
@@ -5469,8 +5854,20 @@
       <c r="I100" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J100">
+        <v>15</v>
+      </c>
+      <c r="K100" t="s">
+        <v>451</v>
+      </c>
+      <c r="L100" s="2">
+        <v>43465</v>
+      </c>
+      <c r="M100" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A101" t="s">
         <v>2</v>
       </c>
@@ -5495,8 +5892,20 @@
       <c r="I101" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J101">
+        <v>95</v>
+      </c>
+      <c r="K101" t="s">
+        <v>453</v>
+      </c>
+      <c r="L101" s="2">
+        <v>43251</v>
+      </c>
+      <c r="M101" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A102" t="s">
         <v>2</v>
       </c>
@@ -5521,8 +5930,20 @@
       <c r="I102" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J102">
+        <v>95</v>
+      </c>
+      <c r="K102" t="s">
+        <v>453</v>
+      </c>
+      <c r="L102" s="2">
+        <v>43251</v>
+      </c>
+      <c r="M102" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="103" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A103" t="s">
         <v>2</v>
       </c>
@@ -5547,8 +5968,20 @@
       <c r="I103" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J103">
+        <v>95</v>
+      </c>
+      <c r="K103" t="s">
+        <v>453</v>
+      </c>
+      <c r="L103" s="2">
+        <v>43251</v>
+      </c>
+      <c r="M103" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="104" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A104" t="s">
         <v>2</v>
       </c>
@@ -5573,8 +6006,20 @@
       <c r="I104" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J104">
+        <v>95</v>
+      </c>
+      <c r="K104" t="s">
+        <v>453</v>
+      </c>
+      <c r="L104" s="2">
+        <v>43251</v>
+      </c>
+      <c r="M104" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="105" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
         <v>2</v>
       </c>
@@ -5599,8 +6044,20 @@
       <c r="I105" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J105">
+        <v>95</v>
+      </c>
+      <c r="K105" t="s">
+        <v>453</v>
+      </c>
+      <c r="L105" s="2">
+        <v>43251</v>
+      </c>
+      <c r="M105" t="s">
+        <v>467</v>
+      </c>
+    </row>
+    <row r="106" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A106" t="s">
         <v>2</v>
       </c>
@@ -5625,8 +6082,20 @@
       <c r="I106" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J106">
+        <v>75</v>
+      </c>
+      <c r="K106" t="s">
+        <v>451</v>
+      </c>
+      <c r="L106" s="2">
+        <v>43344</v>
+      </c>
+      <c r="M106" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
         <v>2</v>
       </c>
@@ -5651,8 +6120,20 @@
       <c r="I107" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J107">
+        <v>75</v>
+      </c>
+      <c r="K107" t="s">
+        <v>451</v>
+      </c>
+      <c r="L107" s="2">
+        <v>43344</v>
+      </c>
+      <c r="M107" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A108" t="s">
         <v>2</v>
       </c>
@@ -5677,8 +6158,20 @@
       <c r="I108" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J108">
+        <v>75</v>
+      </c>
+      <c r="K108" t="s">
+        <v>451</v>
+      </c>
+      <c r="L108" s="2">
+        <v>43344</v>
+      </c>
+      <c r="M108" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="109" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A109" t="s">
         <v>2</v>
       </c>
@@ -5703,8 +6196,20 @@
       <c r="I109" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J109">
+        <v>75</v>
+      </c>
+      <c r="K109" t="s">
+        <v>451</v>
+      </c>
+      <c r="L109" s="2">
+        <v>43344</v>
+      </c>
+      <c r="M109" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="110" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A110" t="s">
         <v>2</v>
       </c>
@@ -5729,8 +6234,20 @@
       <c r="I110" t="s">
         <v>441</v>
       </c>
-    </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J110">
+        <v>75</v>
+      </c>
+      <c r="K110" t="s">
+        <v>451</v>
+      </c>
+      <c r="L110" s="2">
+        <v>43344</v>
+      </c>
+      <c r="M110" t="s">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="111" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
         <v>2</v>
       </c>
@@ -5755,8 +6272,20 @@
       <c r="I111" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J111">
+        <v>95</v>
+      </c>
+      <c r="K111" t="s">
+        <v>451</v>
+      </c>
+      <c r="L111" s="2">
+        <v>43344</v>
+      </c>
+      <c r="M111" t="s">
+        <v>455</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A112" t="s">
         <v>2</v>
       </c>
@@ -5781,6 +6310,18 @@
       <c r="I112" t="s">
         <v>439</v>
       </c>
+      <c r="J112">
+        <v>70</v>
+      </c>
+      <c r="K112" t="s">
+        <v>451</v>
+      </c>
+      <c r="L112" s="2">
+        <v>43344</v>
+      </c>
+      <c r="M112" t="s">
+        <v>468</v>
+      </c>
     </row>
     <row r="113" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
@@ -5807,6 +6348,18 @@
       <c r="I113" t="s">
         <v>439</v>
       </c>
+      <c r="J113">
+        <v>75</v>
+      </c>
+      <c r="K113" t="s">
+        <v>451</v>
+      </c>
+      <c r="L113" s="2">
+        <v>43344</v>
+      </c>
+      <c r="M113" t="s">
+        <v>468</v>
+      </c>
     </row>
     <row r="114" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A114" t="s">
@@ -5833,6 +6386,18 @@
       <c r="I114" t="s">
         <v>434</v>
       </c>
+      <c r="J114">
+        <v>75</v>
+      </c>
+      <c r="K114" t="s">
+        <v>453</v>
+      </c>
+      <c r="L114" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M114" t="s">
+        <v>462</v>
+      </c>
     </row>
     <row r="115" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A115" t="s">
@@ -5859,6 +6424,18 @@
       <c r="I115" t="s">
         <v>439</v>
       </c>
+      <c r="J115">
+        <v>75</v>
+      </c>
+      <c r="K115" t="s">
+        <v>453</v>
+      </c>
+      <c r="L115" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M115" t="s">
+        <v>462</v>
+      </c>
     </row>
     <row r="116" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
@@ -5884,6 +6461,18 @@
       </c>
       <c r="I116" t="s">
         <v>439</v>
+      </c>
+      <c r="J116">
+        <v>75</v>
+      </c>
+      <c r="K116" t="s">
+        <v>453</v>
+      </c>
+      <c r="L116" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M116" t="s">
+        <v>462</v>
       </c>
     </row>
     <row r="117" spans="1:13" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
AOS latency info added
</commit_message>
<xml_diff>
--- a/Latency.xlsx
+++ b/Latency.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kthibault/Documents/GitHub/sandbox/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{D7CA9A5C-3DBF-3C49-AAFC-D2D0F4FAD86E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{78682CB6-CE55-AE49-8FF7-1895C80B4E3F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="1680" windowWidth="35600" windowHeight="18840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9540" yWindow="560" windowWidth="27520" windowHeight="18840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Wait Times" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1940" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2095" uniqueCount="473">
   <si>
     <t>Team</t>
   </si>
@@ -1431,6 +1431,18 @@
   </si>
   <si>
     <t>Awaiting 2017 data - proceeding on schedule; requires final sampling bout for year to be completed; all ticks identified to species; then samples selected for pathogen testing</t>
+  </si>
+  <si>
+    <t>BMI lab processing backlog of samples</t>
+  </si>
+  <si>
+    <t>Waiting on HQ Scientist availability to complete error correction</t>
+  </si>
+  <si>
+    <t>Waiting on field scientist to complete data entry into Fulcrum and HQ scientist to complete QA</t>
+  </si>
+  <si>
+    <t>Waiting for final 2017 data from lab</t>
   </si>
 </sst>
 </file>
@@ -2293,10 +2305,10 @@
   <dimension ref="A1:M260"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="G12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="I190" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O18" sqref="O18"/>
+      <selection pane="bottomRight" activeCell="J207" sqref="J207"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6678,6 +6690,18 @@
       <c r="I122" t="s">
         <v>435</v>
       </c>
+      <c r="J122">
+        <v>90</v>
+      </c>
+      <c r="K122" t="s">
+        <v>453</v>
+      </c>
+      <c r="L122" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M122" t="s">
+        <v>467</v>
+      </c>
     </row>
     <row r="123" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A123" t="s">
@@ -6704,6 +6728,18 @@
       <c r="I123" t="s">
         <v>434</v>
       </c>
+      <c r="J123">
+        <v>90</v>
+      </c>
+      <c r="K123" t="s">
+        <v>453</v>
+      </c>
+      <c r="L123" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M123" t="s">
+        <v>467</v>
+      </c>
     </row>
     <row r="124" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
@@ -6730,6 +6766,12 @@
       <c r="I124" t="s">
         <v>437</v>
       </c>
+      <c r="J124">
+        <v>25</v>
+      </c>
+      <c r="K124" t="s">
+        <v>451</v>
+      </c>
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
@@ -6756,6 +6798,12 @@
       <c r="I125" t="s">
         <v>437</v>
       </c>
+      <c r="J125">
+        <v>25</v>
+      </c>
+      <c r="K125" t="s">
+        <v>451</v>
+      </c>
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
@@ -6782,6 +6830,18 @@
       <c r="I126" t="s">
         <v>435</v>
       </c>
+      <c r="J126">
+        <v>90</v>
+      </c>
+      <c r="K126" t="s">
+        <v>453</v>
+      </c>
+      <c r="L126" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M126" t="s">
+        <v>470</v>
+      </c>
     </row>
     <row r="127" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A127" t="s">
@@ -6808,6 +6868,18 @@
       <c r="I127" t="s">
         <v>434</v>
       </c>
+      <c r="J127">
+        <v>90</v>
+      </c>
+      <c r="K127" t="s">
+        <v>453</v>
+      </c>
+      <c r="L127" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M127" t="s">
+        <v>470</v>
+      </c>
     </row>
     <row r="128" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
@@ -6834,8 +6906,20 @@
       <c r="I128" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J128">
+        <v>90</v>
+      </c>
+      <c r="K128" t="s">
+        <v>453</v>
+      </c>
+      <c r="L128" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M128" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="129" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A129" t="s">
         <v>209</v>
       </c>
@@ -6860,8 +6944,16 @@
       <c r="I129" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J129">
+        <v>25</v>
+      </c>
+      <c r="K129" t="s">
+        <v>451</v>
+      </c>
+      <c r="L129" s="4"/>
+      <c r="M129" s="4"/>
+    </row>
+    <row r="130" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
         <v>209</v>
       </c>
@@ -6886,8 +6978,16 @@
       <c r="I130" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J130">
+        <v>25</v>
+      </c>
+      <c r="K130" t="s">
+        <v>451</v>
+      </c>
+      <c r="L130" s="4"/>
+      <c r="M130" s="4"/>
+    </row>
+    <row r="131" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>209</v>
       </c>
@@ -6912,8 +7012,16 @@
       <c r="I131" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J131">
+        <v>25</v>
+      </c>
+      <c r="K131" t="s">
+        <v>451</v>
+      </c>
+      <c r="L131" s="4"/>
+      <c r="M131" s="4"/>
+    </row>
+    <row r="132" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>209</v>
       </c>
@@ -6938,8 +7046,16 @@
       <c r="I132" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J132">
+        <v>25</v>
+      </c>
+      <c r="K132" t="s">
+        <v>451</v>
+      </c>
+      <c r="L132" s="4"/>
+      <c r="M132" s="4"/>
+    </row>
+    <row r="133" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>209</v>
       </c>
@@ -6964,8 +7080,16 @@
       <c r="I133" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J133">
+        <v>25</v>
+      </c>
+      <c r="K133" t="s">
+        <v>451</v>
+      </c>
+      <c r="L133" s="4"/>
+      <c r="M133" s="4"/>
+    </row>
+    <row r="134" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>209</v>
       </c>
@@ -6990,8 +7114,16 @@
       <c r="I134" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J134">
+        <v>10</v>
+      </c>
+      <c r="K134" t="s">
+        <v>453</v>
+      </c>
+      <c r="L134" s="4"/>
+      <c r="M134" s="4"/>
+    </row>
+    <row r="135" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
         <v>209</v>
       </c>
@@ -7016,8 +7148,16 @@
       <c r="I135" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J135">
+        <v>10</v>
+      </c>
+      <c r="K135" t="s">
+        <v>453</v>
+      </c>
+      <c r="L135" s="4"/>
+      <c r="M135" s="4"/>
+    </row>
+    <row r="136" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
         <v>209</v>
       </c>
@@ -7042,8 +7182,16 @@
       <c r="I136" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J136">
+        <v>10</v>
+      </c>
+      <c r="K136" t="s">
+        <v>453</v>
+      </c>
+      <c r="L136" s="4"/>
+      <c r="M136" s="4"/>
+    </row>
+    <row r="137" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
         <v>209</v>
       </c>
@@ -7068,8 +7216,16 @@
       <c r="I137" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J137">
+        <v>10</v>
+      </c>
+      <c r="K137" t="s">
+        <v>453</v>
+      </c>
+      <c r="L137" s="4"/>
+      <c r="M137" s="4"/>
+    </row>
+    <row r="138" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
         <v>209</v>
       </c>
@@ -7094,8 +7250,20 @@
       <c r="I138" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J138">
+        <v>5</v>
+      </c>
+      <c r="K138" t="s">
+        <v>451</v>
+      </c>
+      <c r="L138" s="2">
+        <v>43435</v>
+      </c>
+      <c r="M138" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="139" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A139" t="s">
         <v>209</v>
       </c>
@@ -7120,8 +7288,20 @@
       <c r="I139" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J139">
+        <v>5</v>
+      </c>
+      <c r="K139" t="s">
+        <v>451</v>
+      </c>
+      <c r="L139" s="2">
+        <v>43435</v>
+      </c>
+      <c r="M139" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="140" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A140" t="s">
         <v>209</v>
       </c>
@@ -7146,8 +7326,20 @@
       <c r="I140" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J140">
+        <v>95</v>
+      </c>
+      <c r="K140" t="s">
+        <v>453</v>
+      </c>
+      <c r="L140" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M140" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="141" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A141" t="s">
         <v>209</v>
       </c>
@@ -7172,8 +7364,20 @@
       <c r="I141" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J141">
+        <v>5</v>
+      </c>
+      <c r="K141" t="s">
+        <v>451</v>
+      </c>
+      <c r="L141" s="2">
+        <v>43435</v>
+      </c>
+      <c r="M141" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="142" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A142" t="s">
         <v>209</v>
       </c>
@@ -7198,8 +7402,20 @@
       <c r="I142" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J142">
+        <v>5</v>
+      </c>
+      <c r="K142" t="s">
+        <v>451</v>
+      </c>
+      <c r="L142" s="2">
+        <v>43435</v>
+      </c>
+      <c r="M142" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="143" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A143" t="s">
         <v>209</v>
       </c>
@@ -7224,8 +7440,20 @@
       <c r="I143" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J143">
+        <v>5</v>
+      </c>
+      <c r="K143" t="s">
+        <v>451</v>
+      </c>
+      <c r="L143" s="2">
+        <v>43435</v>
+      </c>
+      <c r="M143" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="144" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A144" t="s">
         <v>209</v>
       </c>
@@ -7250,8 +7478,20 @@
       <c r="I144" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J144">
+        <v>5</v>
+      </c>
+      <c r="K144" t="s">
+        <v>451</v>
+      </c>
+      <c r="L144" s="2">
+        <v>43435</v>
+      </c>
+      <c r="M144" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="145" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A145" t="s">
         <v>209</v>
       </c>
@@ -7276,8 +7516,20 @@
       <c r="I145" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J145">
+        <v>5</v>
+      </c>
+      <c r="K145" t="s">
+        <v>451</v>
+      </c>
+      <c r="L145" s="2">
+        <v>43435</v>
+      </c>
+      <c r="M145" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="146" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A146" t="s">
         <v>209</v>
       </c>
@@ -7302,8 +7554,20 @@
       <c r="I146" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J146">
+        <v>95</v>
+      </c>
+      <c r="K146" t="s">
+        <v>453</v>
+      </c>
+      <c r="L146" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M146" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="147" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A147" t="s">
         <v>209</v>
       </c>
@@ -7328,8 +7592,20 @@
       <c r="I147" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J147">
+        <v>5</v>
+      </c>
+      <c r="K147" t="s">
+        <v>451</v>
+      </c>
+      <c r="L147" s="2">
+        <v>43435</v>
+      </c>
+      <c r="M147" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="148" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A148" t="s">
         <v>209</v>
       </c>
@@ -7354,8 +7630,20 @@
       <c r="I148" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J148">
+        <v>5</v>
+      </c>
+      <c r="K148" t="s">
+        <v>451</v>
+      </c>
+      <c r="L148" s="2">
+        <v>43435</v>
+      </c>
+      <c r="M148" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="149" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A149" t="s">
         <v>209</v>
       </c>
@@ -7380,8 +7668,20 @@
       <c r="I149" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J149">
+        <v>95</v>
+      </c>
+      <c r="K149" t="s">
+        <v>453</v>
+      </c>
+      <c r="L149" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M149" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="150" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A150" t="s">
         <v>209</v>
       </c>
@@ -7406,8 +7706,20 @@
       <c r="I150" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J150">
+        <v>95</v>
+      </c>
+      <c r="K150" t="s">
+        <v>453</v>
+      </c>
+      <c r="L150" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M150" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="151" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A151" t="s">
         <v>209</v>
       </c>
@@ -7432,8 +7744,20 @@
       <c r="I151" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J151">
+        <v>95</v>
+      </c>
+      <c r="K151" t="s">
+        <v>453</v>
+      </c>
+      <c r="L151" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M151" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="152" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A152" t="s">
         <v>209</v>
       </c>
@@ -7458,8 +7782,20 @@
       <c r="I152" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J152">
+        <v>95</v>
+      </c>
+      <c r="K152" t="s">
+        <v>453</v>
+      </c>
+      <c r="L152" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M152" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="153" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A153" t="s">
         <v>209</v>
       </c>
@@ -7484,8 +7820,20 @@
       <c r="I153" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J153">
+        <v>95</v>
+      </c>
+      <c r="K153" t="s">
+        <v>453</v>
+      </c>
+      <c r="L153" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M153" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="154" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A154" t="s">
         <v>209</v>
       </c>
@@ -7510,8 +7858,20 @@
       <c r="I154" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J154">
+        <v>95</v>
+      </c>
+      <c r="K154" t="s">
+        <v>453</v>
+      </c>
+      <c r="L154" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M154" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="155" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A155" t="s">
         <v>209</v>
       </c>
@@ -7536,8 +7896,20 @@
       <c r="I155" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J155">
+        <v>95</v>
+      </c>
+      <c r="K155" t="s">
+        <v>453</v>
+      </c>
+      <c r="L155" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M155" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="156" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A156" t="s">
         <v>209</v>
       </c>
@@ -7562,8 +7934,20 @@
       <c r="I156" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J156">
+        <v>95</v>
+      </c>
+      <c r="K156" t="s">
+        <v>453</v>
+      </c>
+      <c r="L156" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M156" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="157" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A157" t="s">
         <v>209</v>
       </c>
@@ -7588,8 +7972,17 @@
       <c r="I157" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J157">
+        <v>100</v>
+      </c>
+      <c r="K157" t="s">
+        <v>7</v>
+      </c>
+      <c r="L157" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="158" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A158" t="s">
         <v>209</v>
       </c>
@@ -7614,8 +8007,17 @@
       <c r="I158" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J158">
+        <v>100</v>
+      </c>
+      <c r="K158" t="s">
+        <v>7</v>
+      </c>
+      <c r="L158" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="159" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A159" t="s">
         <v>209</v>
       </c>
@@ -7640,8 +8042,17 @@
       <c r="I159" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J159">
+        <v>100</v>
+      </c>
+      <c r="K159" t="s">
+        <v>7</v>
+      </c>
+      <c r="L159" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="160" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A160" t="s">
         <v>209</v>
       </c>
@@ -7666,8 +8077,17 @@
       <c r="I160" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="161" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J160">
+        <v>100</v>
+      </c>
+      <c r="K160" t="s">
+        <v>7</v>
+      </c>
+      <c r="L160" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="161" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A161" t="s">
         <v>209</v>
       </c>
@@ -7692,8 +8112,17 @@
       <c r="I161" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="162" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J161">
+        <v>100</v>
+      </c>
+      <c r="K161" t="s">
+        <v>7</v>
+      </c>
+      <c r="L161" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="162" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A162" t="s">
         <v>209</v>
       </c>
@@ -7718,8 +8147,17 @@
       <c r="I162" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="163" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J162">
+        <v>100</v>
+      </c>
+      <c r="K162" t="s">
+        <v>7</v>
+      </c>
+      <c r="L162" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="163" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A163" t="s">
         <v>209</v>
       </c>
@@ -7744,8 +8182,17 @@
       <c r="I163" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="164" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J163">
+        <v>100</v>
+      </c>
+      <c r="K163" t="s">
+        <v>7</v>
+      </c>
+      <c r="L163" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="164" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A164" t="s">
         <v>209</v>
       </c>
@@ -7770,8 +8217,20 @@
       <c r="I164" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="165" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J164">
+        <v>10</v>
+      </c>
+      <c r="K164" t="s">
+        <v>453</v>
+      </c>
+      <c r="L164" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M164" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="165" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A165" t="s">
         <v>209</v>
       </c>
@@ -7796,8 +8255,20 @@
       <c r="I165" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="166" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J165">
+        <v>10</v>
+      </c>
+      <c r="K165" t="s">
+        <v>453</v>
+      </c>
+      <c r="L165" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M165" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="166" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A166" t="s">
         <v>209</v>
       </c>
@@ -7822,8 +8293,20 @@
       <c r="I166" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="167" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J166">
+        <v>10</v>
+      </c>
+      <c r="K166" t="s">
+        <v>453</v>
+      </c>
+      <c r="L166" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M166" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="167" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A167" t="s">
         <v>209</v>
       </c>
@@ -7848,8 +8331,20 @@
       <c r="I167" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="168" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J167">
+        <v>10</v>
+      </c>
+      <c r="K167" t="s">
+        <v>453</v>
+      </c>
+      <c r="L167" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M167" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="168" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A168" t="s">
         <v>209</v>
       </c>
@@ -7874,8 +8369,20 @@
       <c r="I168" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="169" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J168">
+        <v>10</v>
+      </c>
+      <c r="K168" t="s">
+        <v>453</v>
+      </c>
+      <c r="L168" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M168" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="169" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A169" t="s">
         <v>209</v>
       </c>
@@ -7900,8 +8407,17 @@
       <c r="I169" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="170" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J169">
+        <v>100</v>
+      </c>
+      <c r="K169" t="s">
+        <v>7</v>
+      </c>
+      <c r="L169" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="170" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A170" t="s">
         <v>209</v>
       </c>
@@ -7926,8 +8442,17 @@
       <c r="I170" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="171" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J170">
+        <v>100</v>
+      </c>
+      <c r="K170" t="s">
+        <v>7</v>
+      </c>
+      <c r="L170" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="171" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A171" t="s">
         <v>209</v>
       </c>
@@ -7952,8 +8477,17 @@
       <c r="I171" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="172" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J171">
+        <v>100</v>
+      </c>
+      <c r="K171" t="s">
+        <v>7</v>
+      </c>
+      <c r="L171" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="172" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A172" t="s">
         <v>209</v>
       </c>
@@ -7978,8 +8512,17 @@
       <c r="I172" t="s">
         <v>439</v>
       </c>
-    </row>
-    <row r="173" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J172">
+        <v>100</v>
+      </c>
+      <c r="K172" t="s">
+        <v>7</v>
+      </c>
+      <c r="L172" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="173" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A173" t="s">
         <v>209</v>
       </c>
@@ -8004,8 +8547,17 @@
       <c r="I173" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="174" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J173">
+        <v>100</v>
+      </c>
+      <c r="K173" t="s">
+        <v>7</v>
+      </c>
+      <c r="L173" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="174" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A174" t="s">
         <v>209</v>
       </c>
@@ -8030,8 +8582,17 @@
       <c r="I174" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="175" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J174">
+        <v>100</v>
+      </c>
+      <c r="K174" t="s">
+        <v>7</v>
+      </c>
+      <c r="L174" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="175" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A175" t="s">
         <v>209</v>
       </c>
@@ -8056,8 +8617,17 @@
       <c r="I175" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="176" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J175">
+        <v>100</v>
+      </c>
+      <c r="K175" t="s">
+        <v>7</v>
+      </c>
+      <c r="L175" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="176" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A176" t="s">
         <v>209</v>
       </c>
@@ -8082,8 +8652,17 @@
       <c r="I176" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J176">
+        <v>100</v>
+      </c>
+      <c r="K176" t="s">
+        <v>7</v>
+      </c>
+      <c r="L176" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="177" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A177" t="s">
         <v>209</v>
       </c>
@@ -8108,8 +8687,20 @@
       <c r="I177" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J177">
+        <v>90</v>
+      </c>
+      <c r="K177" t="s">
+        <v>451</v>
+      </c>
+      <c r="L177" s="2">
+        <v>43312</v>
+      </c>
+      <c r="M177" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="178" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A178" t="s">
         <v>209</v>
       </c>
@@ -8134,8 +8725,20 @@
       <c r="I178" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J178">
+        <v>90</v>
+      </c>
+      <c r="K178" t="s">
+        <v>451</v>
+      </c>
+      <c r="L178" s="2">
+        <v>43312</v>
+      </c>
+      <c r="M178" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="179" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A179" t="s">
         <v>209</v>
       </c>
@@ -8160,8 +8763,17 @@
       <c r="I179" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J179">
+        <v>100</v>
+      </c>
+      <c r="K179" t="s">
+        <v>7</v>
+      </c>
+      <c r="L179" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="180" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A180" t="s">
         <v>209</v>
       </c>
@@ -8186,8 +8798,17 @@
       <c r="I180" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J180">
+        <v>100</v>
+      </c>
+      <c r="K180" t="s">
+        <v>7</v>
+      </c>
+      <c r="L180" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="181" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A181" t="s">
         <v>209</v>
       </c>
@@ -8212,8 +8833,17 @@
       <c r="I181" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J181">
+        <v>100</v>
+      </c>
+      <c r="K181" t="s">
+        <v>7</v>
+      </c>
+      <c r="L181" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="182" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A182" t="s">
         <v>209</v>
       </c>
@@ -8238,8 +8868,16 @@
       <c r="I182" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J182">
+        <v>50</v>
+      </c>
+      <c r="K182" t="s">
+        <v>451</v>
+      </c>
+      <c r="L182" s="4"/>
+      <c r="M182" s="4"/>
+    </row>
+    <row r="183" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
         <v>209</v>
       </c>
@@ -8264,8 +8902,16 @@
       <c r="I183" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J183">
+        <v>50</v>
+      </c>
+      <c r="K183" t="s">
+        <v>451</v>
+      </c>
+      <c r="L183" s="4"/>
+      <c r="M183" s="4"/>
+    </row>
+    <row r="184" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
         <v>209</v>
       </c>
@@ -8290,8 +8936,20 @@
       <c r="I184" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J184">
+        <v>65</v>
+      </c>
+      <c r="K184" t="s">
+        <v>453</v>
+      </c>
+      <c r="L184" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M184" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="185" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A185" t="s">
         <v>209</v>
       </c>
@@ -8316,8 +8974,20 @@
       <c r="I185" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J185">
+        <v>65</v>
+      </c>
+      <c r="K185" t="s">
+        <v>453</v>
+      </c>
+      <c r="L185" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M185" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="186" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A186" t="s">
         <v>209</v>
       </c>
@@ -8342,8 +9012,16 @@
       <c r="I186" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J186">
+        <v>20</v>
+      </c>
+      <c r="K186" t="s">
+        <v>451</v>
+      </c>
+      <c r="L186" s="4"/>
+      <c r="M186" s="4"/>
+    </row>
+    <row r="187" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
         <v>209</v>
       </c>
@@ -8368,8 +9046,16 @@
       <c r="I187" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J187">
+        <v>20</v>
+      </c>
+      <c r="K187" t="s">
+        <v>451</v>
+      </c>
+      <c r="L187" s="4"/>
+      <c r="M187" s="4"/>
+    </row>
+    <row r="188" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
         <v>209</v>
       </c>
@@ -8394,8 +9080,20 @@
       <c r="I188" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J188">
+        <v>90</v>
+      </c>
+      <c r="K188" t="s">
+        <v>453</v>
+      </c>
+      <c r="L188" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M188" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="189" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A189" t="s">
         <v>209</v>
       </c>
@@ -8420,8 +9118,20 @@
       <c r="I189" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J189">
+        <v>90</v>
+      </c>
+      <c r="K189" t="s">
+        <v>453</v>
+      </c>
+      <c r="L189" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M189" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="190" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A190" t="s">
         <v>209</v>
       </c>
@@ -8446,8 +9156,20 @@
       <c r="I190" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J190">
+        <v>90</v>
+      </c>
+      <c r="K190" t="s">
+        <v>453</v>
+      </c>
+      <c r="L190" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M190" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="191" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A191" t="s">
         <v>209</v>
       </c>
@@ -8472,8 +9194,17 @@
       <c r="I191" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J191">
+        <v>100</v>
+      </c>
+      <c r="K191" t="s">
+        <v>7</v>
+      </c>
+      <c r="L191" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="192" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A192" t="s">
         <v>209</v>
       </c>
@@ -8498,8 +9229,17 @@
       <c r="I192" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J192">
+        <v>100</v>
+      </c>
+      <c r="K192" t="s">
+        <v>7</v>
+      </c>
+      <c r="L192" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="193" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A193" t="s">
         <v>209</v>
       </c>
@@ -8524,8 +9264,17 @@
       <c r="I193" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J193">
+        <v>100</v>
+      </c>
+      <c r="K193" t="s">
+        <v>7</v>
+      </c>
+      <c r="L193" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="194" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A194" t="s">
         <v>209</v>
       </c>
@@ -8550,8 +9299,20 @@
       <c r="I194" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J194">
+        <v>90</v>
+      </c>
+      <c r="K194" t="s">
+        <v>453</v>
+      </c>
+      <c r="L194" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M194" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="195" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A195" t="s">
         <v>209</v>
       </c>
@@ -8576,8 +9337,20 @@
       <c r="I195" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J195">
+        <v>90</v>
+      </c>
+      <c r="K195" t="s">
+        <v>453</v>
+      </c>
+      <c r="L195" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M195" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="196" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A196" t="s">
         <v>209</v>
       </c>
@@ -8602,8 +9375,20 @@
       <c r="I196" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J196">
+        <v>90</v>
+      </c>
+      <c r="K196" t="s">
+        <v>453</v>
+      </c>
+      <c r="L196" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M196" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="197" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A197" t="s">
         <v>209</v>
       </c>
@@ -8628,8 +9413,17 @@
       <c r="I197" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J197">
+        <v>100</v>
+      </c>
+      <c r="K197" t="s">
+        <v>7</v>
+      </c>
+      <c r="L197" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="198" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A198" t="s">
         <v>209</v>
       </c>
@@ -8654,8 +9448,17 @@
       <c r="I198" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J198">
+        <v>100</v>
+      </c>
+      <c r="K198" t="s">
+        <v>7</v>
+      </c>
+      <c r="L198" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="199" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A199" t="s">
         <v>209</v>
       </c>
@@ -8680,8 +9483,20 @@
       <c r="I199" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J199">
+        <v>90</v>
+      </c>
+      <c r="K199" t="s">
+        <v>453</v>
+      </c>
+      <c r="L199" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M199" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="200" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A200" t="s">
         <v>209</v>
       </c>
@@ -8706,8 +9521,20 @@
       <c r="I200" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J200">
+        <v>90</v>
+      </c>
+      <c r="K200" t="s">
+        <v>453</v>
+      </c>
+      <c r="L200" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M200" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="201" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A201" t="s">
         <v>209</v>
       </c>
@@ -8732,8 +9559,20 @@
       <c r="I201" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J201">
+        <v>90</v>
+      </c>
+      <c r="K201" t="s">
+        <v>453</v>
+      </c>
+      <c r="L201" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M201" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="202" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A202" t="s">
         <v>209</v>
       </c>
@@ -8758,8 +9597,17 @@
       <c r="I202" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J202">
+        <v>100</v>
+      </c>
+      <c r="K202" t="s">
+        <v>7</v>
+      </c>
+      <c r="L202" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="203" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A203" t="s">
         <v>209</v>
       </c>
@@ -8784,8 +9632,17 @@
       <c r="I203" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J203">
+        <v>100</v>
+      </c>
+      <c r="K203" t="s">
+        <v>7</v>
+      </c>
+      <c r="L203" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="204" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A204" t="s">
         <v>209</v>
       </c>
@@ -8810,8 +9667,20 @@
       <c r="I204" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J204">
+        <v>90</v>
+      </c>
+      <c r="K204" t="s">
+        <v>453</v>
+      </c>
+      <c r="L204" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M204" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="205" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A205" t="s">
         <v>209</v>
       </c>
@@ -8836,8 +9705,20 @@
       <c r="I205" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J205">
+        <v>90</v>
+      </c>
+      <c r="K205" t="s">
+        <v>453</v>
+      </c>
+      <c r="L205" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M205" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="206" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A206" t="s">
         <v>209</v>
       </c>
@@ -8862,8 +9743,17 @@
       <c r="I206" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J206">
+        <v>100</v>
+      </c>
+      <c r="K206" t="s">
+        <v>7</v>
+      </c>
+      <c r="L206" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="207" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A207" t="s">
         <v>209</v>
       </c>
@@ -8889,7 +9779,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
         <v>209</v>
       </c>

</xml_diff>

<commit_message>
first draft of latency data complete; waiting on responses from scientists
</commit_message>
<xml_diff>
--- a/Latency.xlsx
+++ b/Latency.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kthibault/Documents/GitHub/sandbox/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{78682CB6-CE55-AE49-8FF7-1895C80B4E3F}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5053172B-F754-2347-86AA-BCDB855EEFA8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="9540" yWindow="560" windowWidth="27520" windowHeight="18840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2095" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2179" uniqueCount="473">
   <si>
     <t>Team</t>
   </si>
@@ -2305,10 +2305,10 @@
   <dimension ref="A1:M260"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="I190" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J207" sqref="J207"/>
+      <selection pane="bottomRight" activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -9195,13 +9195,16 @@
         <v>437</v>
       </c>
       <c r="J191">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="K191" t="s">
-        <v>7</v>
-      </c>
-      <c r="L191" s="2" t="s">
-        <v>7</v>
+        <v>453</v>
+      </c>
+      <c r="L191" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M191" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="192" spans="1:13" x14ac:dyDescent="0.2">
@@ -9230,13 +9233,16 @@
         <v>437</v>
       </c>
       <c r="J192">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="K192" t="s">
-        <v>7</v>
-      </c>
-      <c r="L192" s="2" t="s">
-        <v>7</v>
+        <v>453</v>
+      </c>
+      <c r="L192" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M192" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="193" spans="1:13" x14ac:dyDescent="0.2">
@@ -9265,13 +9271,16 @@
         <v>434</v>
       </c>
       <c r="J193">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="K193" t="s">
-        <v>7</v>
-      </c>
-      <c r="L193" s="2" t="s">
-        <v>7</v>
+        <v>453</v>
+      </c>
+      <c r="L193" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M193" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="194" spans="1:13" x14ac:dyDescent="0.2">
@@ -9598,13 +9607,16 @@
         <v>437</v>
       </c>
       <c r="J202">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="K202" t="s">
-        <v>7</v>
-      </c>
-      <c r="L202" s="2" t="s">
-        <v>7</v>
+        <v>453</v>
+      </c>
+      <c r="L202" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M202" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="203" spans="1:13" x14ac:dyDescent="0.2">
@@ -9633,13 +9645,16 @@
         <v>434</v>
       </c>
       <c r="J203">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="K203" t="s">
-        <v>7</v>
-      </c>
-      <c r="L203" s="2" t="s">
-        <v>7</v>
+        <v>453</v>
+      </c>
+      <c r="L203" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M203" t="s">
+        <v>470</v>
       </c>
     </row>
     <row r="204" spans="1:13" x14ac:dyDescent="0.2">
@@ -9778,6 +9793,18 @@
       <c r="I207" t="s">
         <v>437</v>
       </c>
+      <c r="J207">
+        <v>90</v>
+      </c>
+      <c r="K207" t="s">
+        <v>453</v>
+      </c>
+      <c r="L207" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M207" t="s">
+        <v>470</v>
+      </c>
     </row>
     <row r="208" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A208" t="s">
@@ -9804,8 +9831,20 @@
       <c r="I208" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J208">
+        <v>90</v>
+      </c>
+      <c r="K208" t="s">
+        <v>453</v>
+      </c>
+      <c r="L208" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M208" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="209" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A209" t="s">
         <v>209</v>
       </c>
@@ -9830,8 +9869,20 @@
       <c r="I209" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J209">
+        <v>90</v>
+      </c>
+      <c r="K209" t="s">
+        <v>453</v>
+      </c>
+      <c r="L209" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M209" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="210" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A210" t="s">
         <v>209</v>
       </c>
@@ -9856,8 +9907,20 @@
       <c r="I210" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J210">
+        <v>90</v>
+      </c>
+      <c r="K210" t="s">
+        <v>453</v>
+      </c>
+      <c r="L210" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M210" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="211" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A211" t="s">
         <v>209</v>
       </c>
@@ -9882,8 +9945,20 @@
       <c r="I211" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J211">
+        <v>90</v>
+      </c>
+      <c r="K211" t="s">
+        <v>453</v>
+      </c>
+      <c r="L211" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M211" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="212" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A212" t="s">
         <v>209</v>
       </c>
@@ -9908,8 +9983,20 @@
       <c r="I212" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J212">
+        <v>90</v>
+      </c>
+      <c r="K212" t="s">
+        <v>453</v>
+      </c>
+      <c r="L212" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M212" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="213" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A213" t="s">
         <v>209</v>
       </c>
@@ -9934,8 +10021,20 @@
       <c r="I213" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J213">
+        <v>90</v>
+      </c>
+      <c r="K213" t="s">
+        <v>453</v>
+      </c>
+      <c r="L213" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M213" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="214" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A214" t="s">
         <v>209</v>
       </c>
@@ -9960,8 +10059,20 @@
       <c r="I214" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J214">
+        <v>90</v>
+      </c>
+      <c r="K214" t="s">
+        <v>453</v>
+      </c>
+      <c r="L214" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M214" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="215" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A215" t="s">
         <v>209</v>
       </c>
@@ -9986,8 +10097,20 @@
       <c r="I215" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J215">
+        <v>90</v>
+      </c>
+      <c r="K215" t="s">
+        <v>453</v>
+      </c>
+      <c r="L215" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M215" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="216" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A216" t="s">
         <v>209</v>
       </c>
@@ -10012,8 +10135,20 @@
       <c r="I216" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J216">
+        <v>90</v>
+      </c>
+      <c r="K216" t="s">
+        <v>453</v>
+      </c>
+      <c r="L216" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M216" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="217" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A217" t="s">
         <v>209</v>
       </c>
@@ -10038,8 +10173,20 @@
       <c r="I217" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J217">
+        <v>90</v>
+      </c>
+      <c r="K217" t="s">
+        <v>453</v>
+      </c>
+      <c r="L217" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M217" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="218" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A218" t="s">
         <v>209</v>
       </c>
@@ -10064,8 +10211,15 @@
       <c r="I218" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J218">
+        <v>80</v>
+      </c>
+      <c r="K218" t="s">
+        <v>451</v>
+      </c>
+      <c r="L218" s="4"/>
+    </row>
+    <row r="219" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
         <v>209</v>
       </c>
@@ -10090,8 +10244,17 @@
       <c r="I219" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J219">
+        <v>100</v>
+      </c>
+      <c r="K219" t="s">
+        <v>7</v>
+      </c>
+      <c r="L219" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="220" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A220" t="s">
         <v>209</v>
       </c>
@@ -10116,8 +10279,17 @@
       <c r="I220" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J220">
+        <v>100</v>
+      </c>
+      <c r="K220" t="s">
+        <v>7</v>
+      </c>
+      <c r="L220" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="221" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A221" t="s">
         <v>209</v>
       </c>
@@ -10142,8 +10314,17 @@
       <c r="I221" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J221">
+        <v>100</v>
+      </c>
+      <c r="K221" t="s">
+        <v>7</v>
+      </c>
+      <c r="L221" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="222" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A222" t="s">
         <v>209</v>
       </c>
@@ -10168,8 +10349,16 @@
       <c r="I222" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J222" s="4">
+        <v>10</v>
+      </c>
+      <c r="K222" s="4" t="s">
+        <v>453</v>
+      </c>
+      <c r="L222" s="4"/>
+      <c r="M222" s="4"/>
+    </row>
+    <row r="223" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
         <v>209</v>
       </c>
@@ -10194,8 +10383,12 @@
       <c r="I223" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J223" s="4"/>
+      <c r="K223" s="4"/>
+      <c r="L223" s="4"/>
+      <c r="M223" s="4"/>
+    </row>
+    <row r="224" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
         <v>209</v>
       </c>
@@ -10220,8 +10413,12 @@
       <c r="I224" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J224" s="4"/>
+      <c r="K224" s="4"/>
+      <c r="L224" s="4"/>
+      <c r="M224" s="4"/>
+    </row>
+    <row r="225" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
         <v>209</v>
       </c>
@@ -10246,8 +10443,12 @@
       <c r="I225" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J225" s="4"/>
+      <c r="K225" s="4"/>
+      <c r="L225" s="4"/>
+      <c r="M225" s="4"/>
+    </row>
+    <row r="226" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
         <v>209</v>
       </c>
@@ -10272,8 +10473,12 @@
       <c r="I226" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J226" s="4"/>
+      <c r="K226" s="4"/>
+      <c r="L226" s="4"/>
+      <c r="M226" s="4"/>
+    </row>
+    <row r="227" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
         <v>209</v>
       </c>
@@ -10298,8 +10503,12 @@
       <c r="I227" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J227" s="4"/>
+      <c r="K227" s="4"/>
+      <c r="L227" s="4"/>
+      <c r="M227" s="4"/>
+    </row>
+    <row r="228" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
         <v>209</v>
       </c>
@@ -10324,8 +10533,12 @@
       <c r="I228" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J228" s="4"/>
+      <c r="K228" s="4"/>
+      <c r="L228" s="4"/>
+      <c r="M228" s="4"/>
+    </row>
+    <row r="229" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
         <v>209</v>
       </c>
@@ -10350,8 +10563,12 @@
       <c r="I229" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J229" s="4"/>
+      <c r="K229" s="4"/>
+      <c r="L229" s="4"/>
+      <c r="M229" s="4"/>
+    </row>
+    <row r="230" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
         <v>209</v>
       </c>
@@ -10376,8 +10593,12 @@
       <c r="I230" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J230" s="4"/>
+      <c r="K230" s="4"/>
+      <c r="L230" s="4"/>
+      <c r="M230" s="4"/>
+    </row>
+    <row r="231" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
         <v>209</v>
       </c>
@@ -10402,8 +10623,12 @@
       <c r="I231" t="s">
         <v>435</v>
       </c>
-    </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J231" s="4"/>
+      <c r="K231" s="4"/>
+      <c r="L231" s="4"/>
+      <c r="M231" s="4"/>
+    </row>
+    <row r="232" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
         <v>209</v>
       </c>
@@ -10428,8 +10653,20 @@
       <c r="I232" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J232">
+        <v>95</v>
+      </c>
+      <c r="K232" t="s">
+        <v>453</v>
+      </c>
+      <c r="L232" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M232" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="233" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A233" t="s">
         <v>209</v>
       </c>
@@ -10454,8 +10691,20 @@
       <c r="I233" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J233">
+        <v>95</v>
+      </c>
+      <c r="K233" t="s">
+        <v>453</v>
+      </c>
+      <c r="L233" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M233" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="234" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A234" t="s">
         <v>209</v>
       </c>
@@ -10480,8 +10729,20 @@
       <c r="I234" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J234">
+        <v>95</v>
+      </c>
+      <c r="K234" t="s">
+        <v>453</v>
+      </c>
+      <c r="L234" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M234" t="s">
+        <v>470</v>
+      </c>
+    </row>
+    <row r="235" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A235" t="s">
         <v>209</v>
       </c>
@@ -10506,8 +10767,20 @@
       <c r="I235" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J235">
+        <v>5</v>
+      </c>
+      <c r="K235" t="s">
+        <v>451</v>
+      </c>
+      <c r="L235" s="2">
+        <v>43435</v>
+      </c>
+      <c r="M235" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="236" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A236" t="s">
         <v>209</v>
       </c>
@@ -10532,8 +10805,20 @@
       <c r="I236" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J236">
+        <v>5</v>
+      </c>
+      <c r="K236" t="s">
+        <v>451</v>
+      </c>
+      <c r="L236" s="2">
+        <v>43435</v>
+      </c>
+      <c r="M236" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="237" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A237" t="s">
         <v>209</v>
       </c>
@@ -10558,8 +10843,20 @@
       <c r="I237" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J237">
+        <v>5</v>
+      </c>
+      <c r="K237" t="s">
+        <v>451</v>
+      </c>
+      <c r="L237" s="2">
+        <v>43435</v>
+      </c>
+      <c r="M237" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="238" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A238" t="s">
         <v>209</v>
       </c>
@@ -10584,8 +10881,20 @@
       <c r="I238" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J238">
+        <v>5</v>
+      </c>
+      <c r="K238" t="s">
+        <v>451</v>
+      </c>
+      <c r="L238" s="2">
+        <v>43435</v>
+      </c>
+      <c r="M238" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="239" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A239" t="s">
         <v>209</v>
       </c>
@@ -10610,8 +10919,20 @@
       <c r="I239" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="240" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J239">
+        <v>5</v>
+      </c>
+      <c r="K239" t="s">
+        <v>451</v>
+      </c>
+      <c r="L239" s="2">
+        <v>43435</v>
+      </c>
+      <c r="M239" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="240" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A240" t="s">
         <v>209</v>
       </c>
@@ -10636,8 +10957,20 @@
       <c r="I240" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="241" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J240">
+        <v>5</v>
+      </c>
+      <c r="K240" t="s">
+        <v>451</v>
+      </c>
+      <c r="L240" s="2">
+        <v>43435</v>
+      </c>
+      <c r="M240" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="241" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A241" t="s">
         <v>209</v>
       </c>
@@ -10662,8 +10995,20 @@
       <c r="I241" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="242" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J241">
+        <v>5</v>
+      </c>
+      <c r="K241" t="s">
+        <v>451</v>
+      </c>
+      <c r="L241" s="2">
+        <v>43435</v>
+      </c>
+      <c r="M241" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="242" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A242" t="s">
         <v>209</v>
       </c>
@@ -10688,8 +11033,20 @@
       <c r="I242" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="243" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J242">
+        <v>5</v>
+      </c>
+      <c r="K242" t="s">
+        <v>451</v>
+      </c>
+      <c r="L242" s="2">
+        <v>43435</v>
+      </c>
+      <c r="M242" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="243" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A243" t="s">
         <v>209</v>
       </c>
@@ -10714,8 +11071,20 @@
       <c r="I243" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="244" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J243">
+        <v>5</v>
+      </c>
+      <c r="K243" t="s">
+        <v>451</v>
+      </c>
+      <c r="L243" s="2">
+        <v>43435</v>
+      </c>
+      <c r="M243" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="244" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A244" t="s">
         <v>209</v>
       </c>
@@ -10740,8 +11109,20 @@
       <c r="I244" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="245" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J244">
+        <v>5</v>
+      </c>
+      <c r="K244" t="s">
+        <v>451</v>
+      </c>
+      <c r="L244" s="2">
+        <v>43435</v>
+      </c>
+      <c r="M244" t="s">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="245" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A245" t="s">
         <v>209</v>
       </c>
@@ -10766,8 +11147,16 @@
       <c r="I245" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="246" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J245">
+        <v>90</v>
+      </c>
+      <c r="K245" t="s">
+        <v>451</v>
+      </c>
+      <c r="L245" s="4"/>
+      <c r="M245" s="4"/>
+    </row>
+    <row r="246" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
         <v>209</v>
       </c>
@@ -10792,8 +11181,16 @@
       <c r="I246" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="247" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J246">
+        <v>90</v>
+      </c>
+      <c r="K246" t="s">
+        <v>451</v>
+      </c>
+      <c r="L246" s="4"/>
+      <c r="M246" s="4"/>
+    </row>
+    <row r="247" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
         <v>209</v>
       </c>
@@ -10818,8 +11215,16 @@
       <c r="I247" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="248" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J247">
+        <v>90</v>
+      </c>
+      <c r="K247" t="s">
+        <v>451</v>
+      </c>
+      <c r="L247" s="4"/>
+      <c r="M247" s="4"/>
+    </row>
+    <row r="248" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
         <v>209</v>
       </c>
@@ -10844,8 +11249,16 @@
       <c r="I248" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="249" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J248">
+        <v>90</v>
+      </c>
+      <c r="K248" t="s">
+        <v>451</v>
+      </c>
+      <c r="L248" s="4"/>
+      <c r="M248" s="4"/>
+    </row>
+    <row r="249" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
         <v>209</v>
       </c>
@@ -10870,8 +11283,17 @@
       <c r="I249" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="250" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J249">
+        <v>100</v>
+      </c>
+      <c r="K249" t="s">
+        <v>7</v>
+      </c>
+      <c r="L249" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="250" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A250" t="s">
         <v>209</v>
       </c>
@@ -10896,8 +11318,17 @@
       <c r="I250" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="251" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J250">
+        <v>100</v>
+      </c>
+      <c r="K250" t="s">
+        <v>7</v>
+      </c>
+      <c r="L250" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="251" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A251" t="s">
         <v>209</v>
       </c>
@@ -10922,8 +11353,17 @@
       <c r="I251" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="252" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J251">
+        <v>100</v>
+      </c>
+      <c r="K251" t="s">
+        <v>7</v>
+      </c>
+      <c r="L251" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="252" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A252" t="s">
         <v>411</v>
       </c>
@@ -10948,8 +11388,17 @@
       <c r="I252" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="253" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J252">
+        <v>100</v>
+      </c>
+      <c r="K252" t="s">
+        <v>7</v>
+      </c>
+      <c r="L252" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="253" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A253" t="s">
         <v>411</v>
       </c>
@@ -10974,8 +11423,17 @@
       <c r="I253" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="254" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J253">
+        <v>100</v>
+      </c>
+      <c r="K253" t="s">
+        <v>7</v>
+      </c>
+      <c r="L253" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="254" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A254" t="s">
         <v>411</v>
       </c>
@@ -11000,8 +11458,17 @@
       <c r="I254" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="255" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J254">
+        <v>100</v>
+      </c>
+      <c r="K254" t="s">
+        <v>7</v>
+      </c>
+      <c r="L254" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="255" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A255" t="s">
         <v>411</v>
       </c>
@@ -11026,8 +11493,17 @@
       <c r="I255" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="256" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J255">
+        <v>100</v>
+      </c>
+      <c r="K255" t="s">
+        <v>7</v>
+      </c>
+      <c r="L255" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="256" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A256" t="s">
         <v>411</v>
       </c>
@@ -11052,8 +11528,17 @@
       <c r="I256" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="257" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J256">
+        <v>100</v>
+      </c>
+      <c r="K256" t="s">
+        <v>7</v>
+      </c>
+      <c r="L256" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="257" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A257" t="s">
         <v>411</v>
       </c>
@@ -11078,8 +11563,17 @@
       <c r="I257" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="258" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J257">
+        <v>100</v>
+      </c>
+      <c r="K257" t="s">
+        <v>7</v>
+      </c>
+      <c r="L257" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="258" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A258" t="s">
         <v>411</v>
       </c>
@@ -11104,8 +11598,17 @@
       <c r="I258" t="s">
         <v>437</v>
       </c>
-    </row>
-    <row r="259" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J258">
+        <v>100</v>
+      </c>
+      <c r="K258" t="s">
+        <v>7</v>
+      </c>
+      <c r="L258" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="259" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A259" t="s">
         <v>411</v>
       </c>
@@ -11130,8 +11633,17 @@
       <c r="I259" t="s">
         <v>434</v>
       </c>
-    </row>
-    <row r="260" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="J259">
+        <v>100</v>
+      </c>
+      <c r="K259" t="s">
+        <v>7</v>
+      </c>
+      <c r="L259" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="260" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A260" t="s">
         <v>411</v>
       </c>
@@ -11155,6 +11667,15 @@
       </c>
       <c r="I260" t="s">
         <v>437</v>
+      </c>
+      <c r="J260">
+        <v>100</v>
+      </c>
+      <c r="K260" t="s">
+        <v>7</v>
+      </c>
+      <c r="L260" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
completed latency data file
</commit_message>
<xml_diff>
--- a/Latency.xlsx
+++ b/Latency.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10513"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kthibault/Documents/GitHub/sandbox/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{5053172B-F754-2347-86AA-BCDB855EEFA8}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{78E8122F-1D0A-FC46-AA1F-952C9AEC7C21}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9540" yWindow="560" windowWidth="27520" windowHeight="18840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1240" yWindow="2060" windowWidth="28660" windowHeight="17860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Wait Times" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2179" uniqueCount="473">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2235" uniqueCount="478">
   <si>
     <t>Team</t>
   </si>
@@ -1443,6 +1443,21 @@
   </si>
   <si>
     <t>Waiting for final 2017 data from lab</t>
+  </si>
+  <si>
+    <t>Drexel lab contractually has until June 30 to return data</t>
+  </si>
+  <si>
+    <t>Lab contractually has until June 30 to return data</t>
+  </si>
+  <si>
+    <t>SIRFIR lab contractually has until June 30 to return data</t>
+  </si>
+  <si>
+    <t>Waiting on HQ Scientist availability to process data to generate maps</t>
+  </si>
+  <si>
+    <t>EcoCore not returning data on time; samples backlogged</t>
   </si>
 </sst>
 </file>
@@ -1592,7 +1607,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1772,12 +1787,6 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -1939,14 +1948,15 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2305,10 +2315,10 @@
   <dimension ref="A1:M260"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <pane xSplit="4" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L11" sqref="L11"/>
+      <selection pane="bottomRight" activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2742,7 +2752,7 @@
         <v>450</v>
       </c>
       <c r="L12" s="2">
-        <v>43374</v>
+        <v>43404</v>
       </c>
       <c r="M12" t="s">
         <v>452</v>
@@ -2780,7 +2790,7 @@
         <v>450</v>
       </c>
       <c r="L13" s="2">
-        <v>43374</v>
+        <v>43404</v>
       </c>
       <c r="M13" t="s">
         <v>452</v>
@@ -2818,7 +2828,7 @@
         <v>450</v>
       </c>
       <c r="L14" s="2">
-        <v>43374</v>
+        <v>43404</v>
       </c>
       <c r="M14" t="s">
         <v>452</v>
@@ -2856,7 +2866,7 @@
         <v>450</v>
       </c>
       <c r="L15" s="2">
-        <v>43374</v>
+        <v>43404</v>
       </c>
       <c r="M15" t="s">
         <v>452</v>
@@ -2929,7 +2939,7 @@
         <v>450</v>
       </c>
       <c r="L17" s="2">
-        <v>43374</v>
+        <v>43404</v>
       </c>
       <c r="M17" t="s">
         <v>452</v>
@@ -2967,7 +2977,7 @@
         <v>450</v>
       </c>
       <c r="L18" s="2">
-        <v>43374</v>
+        <v>43404</v>
       </c>
       <c r="M18" t="s">
         <v>452</v>
@@ -3186,7 +3196,7 @@
         <v>451</v>
       </c>
       <c r="L24" s="2">
-        <v>43344</v>
+        <v>43373</v>
       </c>
       <c r="M24" t="s">
         <v>455</v>
@@ -3259,7 +3269,7 @@
         <v>451</v>
       </c>
       <c r="L26" s="2">
-        <v>43344</v>
+        <v>43373</v>
       </c>
       <c r="M26" t="s">
         <v>455</v>
@@ -3437,7 +3447,7 @@
         <v>450</v>
       </c>
       <c r="L31" s="2">
-        <v>43374</v>
+        <v>43404</v>
       </c>
       <c r="M31" t="s">
         <v>452</v>
@@ -3475,7 +3485,7 @@
         <v>450</v>
       </c>
       <c r="L32" s="2">
-        <v>43374</v>
+        <v>43404</v>
       </c>
       <c r="M32" t="s">
         <v>452</v>
@@ -3513,7 +3523,7 @@
         <v>450</v>
       </c>
       <c r="L33" s="2">
-        <v>43374</v>
+        <v>43404</v>
       </c>
       <c r="M33" t="s">
         <v>452</v>
@@ -3551,7 +3561,7 @@
         <v>450</v>
       </c>
       <c r="L34" s="2">
-        <v>43374</v>
+        <v>43404</v>
       </c>
       <c r="M34" t="s">
         <v>452</v>
@@ -3589,7 +3599,7 @@
         <v>450</v>
       </c>
       <c r="L35" s="2">
-        <v>43435</v>
+        <v>43465</v>
       </c>
       <c r="M35" t="s">
         <v>452</v>
@@ -3627,7 +3637,7 @@
         <v>450</v>
       </c>
       <c r="L36" s="2">
-        <v>43435</v>
+        <v>43465</v>
       </c>
       <c r="M36" t="s">
         <v>452</v>
@@ -3703,7 +3713,7 @@
         <v>450</v>
       </c>
       <c r="L38" s="2">
-        <v>43435</v>
+        <v>43465</v>
       </c>
       <c r="M38" t="s">
         <v>452</v>
@@ -3881,7 +3891,7 @@
         <v>457</v>
       </c>
       <c r="L43" s="2">
-        <v>43435</v>
+        <v>43465</v>
       </c>
       <c r="M43" t="s">
         <v>461</v>
@@ -4143,7 +4153,7 @@
         <v>451</v>
       </c>
       <c r="L51" s="2">
-        <v>43344</v>
+        <v>43373</v>
       </c>
       <c r="M51" t="s">
         <v>455</v>
@@ -4443,7 +4453,7 @@
         <v>451</v>
       </c>
       <c r="L60" s="2">
-        <v>43344</v>
+        <v>43373</v>
       </c>
       <c r="M60" t="s">
         <v>455</v>
@@ -4481,7 +4491,7 @@
         <v>451</v>
       </c>
       <c r="L61" s="2">
-        <v>43344</v>
+        <v>43373</v>
       </c>
       <c r="M61" t="s">
         <v>464</v>
@@ -4519,7 +4529,7 @@
         <v>451</v>
       </c>
       <c r="L62" s="2">
-        <v>43344</v>
+        <v>43373</v>
       </c>
       <c r="M62" t="s">
         <v>464</v>
@@ -4557,7 +4567,7 @@
         <v>451</v>
       </c>
       <c r="L63" s="2">
-        <v>43344</v>
+        <v>43373</v>
       </c>
       <c r="M63" t="s">
         <v>464</v>
@@ -4735,7 +4745,7 @@
         <v>451</v>
       </c>
       <c r="L68" s="2">
-        <v>43344</v>
+        <v>43373</v>
       </c>
       <c r="M68" t="s">
         <v>455</v>
@@ -4869,7 +4879,7 @@
         <v>450</v>
       </c>
       <c r="L72" s="2">
-        <v>43374</v>
+        <v>43404</v>
       </c>
       <c r="M72" t="s">
         <v>452</v>
@@ -4907,7 +4917,7 @@
         <v>450</v>
       </c>
       <c r="L73" s="2">
-        <v>43374</v>
+        <v>43404</v>
       </c>
       <c r="M73" t="s">
         <v>452</v>
@@ -4945,7 +4955,7 @@
         <v>450</v>
       </c>
       <c r="L74" s="2">
-        <v>43374</v>
+        <v>43404</v>
       </c>
       <c r="M74" t="s">
         <v>452</v>
@@ -4983,7 +4993,7 @@
         <v>450</v>
       </c>
       <c r="L75" s="2">
-        <v>43374</v>
+        <v>43404</v>
       </c>
       <c r="M75" t="s">
         <v>452</v>
@@ -5059,7 +5069,7 @@
         <v>451</v>
       </c>
       <c r="L77" s="2">
-        <v>43344</v>
+        <v>43373</v>
       </c>
       <c r="M77" t="s">
         <v>455</v>
@@ -5097,7 +5107,7 @@
         <v>451</v>
       </c>
       <c r="L78" s="2">
-        <v>43344</v>
+        <v>43373</v>
       </c>
       <c r="M78" t="s">
         <v>463</v>
@@ -5135,7 +5145,7 @@
         <v>451</v>
       </c>
       <c r="L79" s="2">
-        <v>43344</v>
+        <v>43373</v>
       </c>
       <c r="M79" t="s">
         <v>463</v>
@@ -5173,7 +5183,7 @@
         <v>451</v>
       </c>
       <c r="L80" s="2">
-        <v>43344</v>
+        <v>43373</v>
       </c>
       <c r="M80" t="s">
         <v>463</v>
@@ -5211,7 +5221,7 @@
         <v>451</v>
       </c>
       <c r="L81" s="2">
-        <v>43344</v>
+        <v>43373</v>
       </c>
       <c r="M81" t="s">
         <v>463</v>
@@ -5248,8 +5258,12 @@
       <c r="K82" t="s">
         <v>451</v>
       </c>
-      <c r="L82" s="4"/>
-      <c r="M82" s="4"/>
+      <c r="L82" s="2">
+        <v>43373</v>
+      </c>
+      <c r="M82" s="4" t="s">
+        <v>477</v>
+      </c>
     </row>
     <row r="83" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
@@ -5282,8 +5296,12 @@
       <c r="K83" t="s">
         <v>451</v>
       </c>
-      <c r="L83" s="4"/>
-      <c r="M83" s="4"/>
+      <c r="L83" s="2">
+        <v>43373</v>
+      </c>
+      <c r="M83" s="4" t="s">
+        <v>477</v>
+      </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A84" t="s">
@@ -5316,8 +5334,12 @@
       <c r="K84" t="s">
         <v>451</v>
       </c>
-      <c r="L84" s="4"/>
-      <c r="M84" s="4"/>
+      <c r="L84" s="2">
+        <v>43373</v>
+      </c>
+      <c r="M84" s="4" t="s">
+        <v>477</v>
+      </c>
     </row>
     <row r="85" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A85" t="s">
@@ -5350,8 +5372,12 @@
       <c r="K85" t="s">
         <v>451</v>
       </c>
-      <c r="L85" s="4"/>
-      <c r="M85" s="4"/>
+      <c r="L85" s="5">
+        <v>43343</v>
+      </c>
+      <c r="M85" s="4" t="s">
+        <v>477</v>
+      </c>
     </row>
     <row r="86" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A86" t="s">
@@ -5384,8 +5410,12 @@
       <c r="K86" t="s">
         <v>451</v>
       </c>
-      <c r="L86" s="4"/>
-      <c r="M86" s="4"/>
+      <c r="L86" s="5">
+        <v>43343</v>
+      </c>
+      <c r="M86" s="4" t="s">
+        <v>477</v>
+      </c>
     </row>
     <row r="87" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A87" t="s">
@@ -5418,8 +5448,12 @@
       <c r="K87" t="s">
         <v>451</v>
       </c>
-      <c r="L87" s="4"/>
-      <c r="M87" s="4"/>
+      <c r="L87" s="2">
+        <v>43465</v>
+      </c>
+      <c r="M87" t="s">
+        <v>469</v>
+      </c>
     </row>
     <row r="88" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A88" t="s">
@@ -5452,8 +5486,12 @@
       <c r="K88" t="s">
         <v>451</v>
       </c>
-      <c r="L88" s="4"/>
-      <c r="M88" s="4"/>
+      <c r="L88" s="2">
+        <v>43465</v>
+      </c>
+      <c r="M88" t="s">
+        <v>469</v>
+      </c>
     </row>
     <row r="89" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A89" t="s">
@@ -5486,8 +5524,12 @@
       <c r="K89" t="s">
         <v>451</v>
       </c>
-      <c r="L89" s="4"/>
-      <c r="M89" s="4"/>
+      <c r="L89" s="2">
+        <v>43465</v>
+      </c>
+      <c r="M89" t="s">
+        <v>469</v>
+      </c>
     </row>
     <row r="90" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
@@ -5520,8 +5562,12 @@
       <c r="K90" t="s">
         <v>451</v>
       </c>
-      <c r="L90" s="4"/>
-      <c r="M90" s="4"/>
+      <c r="L90" s="2">
+        <v>43465</v>
+      </c>
+      <c r="M90" t="s">
+        <v>469</v>
+      </c>
     </row>
     <row r="91" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A91" t="s">
@@ -5554,8 +5600,12 @@
       <c r="K91" t="s">
         <v>451</v>
       </c>
-      <c r="L91" s="4"/>
-      <c r="M91" s="4"/>
+      <c r="L91" s="2">
+        <v>43465</v>
+      </c>
+      <c r="M91" t="s">
+        <v>469</v>
+      </c>
     </row>
     <row r="92" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
@@ -5588,8 +5638,12 @@
       <c r="K92" t="s">
         <v>451</v>
       </c>
-      <c r="L92" s="4"/>
-      <c r="M92" s="4"/>
+      <c r="L92" s="2">
+        <v>43465</v>
+      </c>
+      <c r="M92" t="s">
+        <v>469</v>
+      </c>
     </row>
     <row r="93" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
@@ -5622,8 +5676,12 @@
       <c r="K93" t="s">
         <v>451</v>
       </c>
-      <c r="L93" s="4"/>
-      <c r="M93" s="4"/>
+      <c r="L93" s="2">
+        <v>43465</v>
+      </c>
+      <c r="M93" t="s">
+        <v>469</v>
+      </c>
     </row>
     <row r="94" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
@@ -5656,8 +5714,12 @@
       <c r="K94" t="s">
         <v>451</v>
       </c>
-      <c r="L94" s="4"/>
-      <c r="M94" s="4"/>
+      <c r="L94" s="2">
+        <v>43465</v>
+      </c>
+      <c r="M94" t="s">
+        <v>469</v>
+      </c>
     </row>
     <row r="95" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
@@ -5690,8 +5752,12 @@
       <c r="K95" t="s">
         <v>451</v>
       </c>
-      <c r="L95" s="4"/>
-      <c r="M95" s="4"/>
+      <c r="L95" s="2">
+        <v>43465</v>
+      </c>
+      <c r="M95" t="s">
+        <v>469</v>
+      </c>
     </row>
     <row r="96" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A96" t="s">
@@ -5724,8 +5790,12 @@
       <c r="K96" t="s">
         <v>451</v>
       </c>
-      <c r="L96" s="4"/>
-      <c r="M96" s="4"/>
+      <c r="L96" s="2">
+        <v>43465</v>
+      </c>
+      <c r="M96" t="s">
+        <v>469</v>
+      </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
@@ -6101,7 +6171,7 @@
         <v>451</v>
       </c>
       <c r="L106" s="2">
-        <v>43344</v>
+        <v>43373</v>
       </c>
       <c r="M106" t="s">
         <v>463</v>
@@ -6139,7 +6209,7 @@
         <v>451</v>
       </c>
       <c r="L107" s="2">
-        <v>43344</v>
+        <v>43373</v>
       </c>
       <c r="M107" t="s">
         <v>463</v>
@@ -6177,7 +6247,7 @@
         <v>451</v>
       </c>
       <c r="L108" s="2">
-        <v>43344</v>
+        <v>43373</v>
       </c>
       <c r="M108" t="s">
         <v>463</v>
@@ -6215,7 +6285,7 @@
         <v>451</v>
       </c>
       <c r="L109" s="2">
-        <v>43344</v>
+        <v>43373</v>
       </c>
       <c r="M109" t="s">
         <v>463</v>
@@ -6253,7 +6323,7 @@
         <v>451</v>
       </c>
       <c r="L110" s="2">
-        <v>43344</v>
+        <v>43373</v>
       </c>
       <c r="M110" t="s">
         <v>463</v>
@@ -6291,7 +6361,7 @@
         <v>451</v>
       </c>
       <c r="L111" s="2">
-        <v>43344</v>
+        <v>43373</v>
       </c>
       <c r="M111" t="s">
         <v>455</v>
@@ -6329,7 +6399,7 @@
         <v>451</v>
       </c>
       <c r="L112" s="2">
-        <v>43344</v>
+        <v>43373</v>
       </c>
       <c r="M112" t="s">
         <v>468</v>
@@ -6367,7 +6437,7 @@
         <v>451</v>
       </c>
       <c r="L113" s="2">
-        <v>43344</v>
+        <v>43373</v>
       </c>
       <c r="M113" t="s">
         <v>468</v>
@@ -6519,7 +6589,7 @@
         <v>457</v>
       </c>
       <c r="L117" s="2">
-        <v>43435</v>
+        <v>43465</v>
       </c>
       <c r="M117" t="s">
         <v>458</v>
@@ -6557,7 +6627,7 @@
         <v>457</v>
       </c>
       <c r="L118" s="2">
-        <v>43435</v>
+        <v>43465</v>
       </c>
       <c r="M118" t="s">
         <v>458</v>
@@ -6595,7 +6665,7 @@
         <v>457</v>
       </c>
       <c r="L119" s="2">
-        <v>43435</v>
+        <v>43465</v>
       </c>
       <c r="M119" t="s">
         <v>458</v>
@@ -6633,7 +6703,7 @@
         <v>457</v>
       </c>
       <c r="L120" s="2">
-        <v>43435</v>
+        <v>43465</v>
       </c>
       <c r="M120" t="s">
         <v>458</v>
@@ -6664,6 +6734,18 @@
       <c r="I121" t="s">
         <v>437</v>
       </c>
+      <c r="J121">
+        <v>70</v>
+      </c>
+      <c r="K121" t="s">
+        <v>451</v>
+      </c>
+      <c r="L121" s="2">
+        <v>43312</v>
+      </c>
+      <c r="M121" s="4" t="s">
+        <v>475</v>
+      </c>
     </row>
     <row r="122" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A122" t="s">
@@ -6772,6 +6854,12 @@
       <c r="K124" t="s">
         <v>451</v>
       </c>
+      <c r="L124" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M124" s="4" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="125" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
@@ -6804,6 +6892,12 @@
       <c r="K125" t="s">
         <v>451</v>
       </c>
+      <c r="L125" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M125" s="4" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="126" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A126" t="s">
@@ -6950,8 +7044,12 @@
       <c r="K129" t="s">
         <v>451</v>
       </c>
-      <c r="L129" s="4"/>
-      <c r="M129" s="4"/>
+      <c r="L129" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M129" s="4" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="130" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A130" t="s">
@@ -6984,8 +7082,12 @@
       <c r="K130" t="s">
         <v>451</v>
       </c>
-      <c r="L130" s="4"/>
-      <c r="M130" s="4"/>
+      <c r="L130" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M130" s="4" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="131" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
@@ -7018,8 +7120,12 @@
       <c r="K131" t="s">
         <v>451</v>
       </c>
-      <c r="L131" s="4"/>
-      <c r="M131" s="4"/>
+      <c r="L131" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M131" s="4" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="132" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
@@ -7052,8 +7158,12 @@
       <c r="K132" t="s">
         <v>451</v>
       </c>
-      <c r="L132" s="4"/>
-      <c r="M132" s="4"/>
+      <c r="L132" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M132" s="4" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="133" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
@@ -7086,8 +7196,12 @@
       <c r="K133" t="s">
         <v>451</v>
       </c>
-      <c r="L133" s="4"/>
-      <c r="M133" s="4"/>
+      <c r="L133" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M133" s="4" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="134" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
@@ -7120,8 +7234,12 @@
       <c r="K134" t="s">
         <v>453</v>
       </c>
-      <c r="L134" s="4"/>
-      <c r="M134" s="4"/>
+      <c r="L134" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M134" s="4" t="s">
+        <v>476</v>
+      </c>
     </row>
     <row r="135" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A135" t="s">
@@ -7154,8 +7272,12 @@
       <c r="K135" t="s">
         <v>453</v>
       </c>
-      <c r="L135" s="4"/>
-      <c r="M135" s="4"/>
+      <c r="L135" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M135" s="4" t="s">
+        <v>476</v>
+      </c>
     </row>
     <row r="136" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A136" t="s">
@@ -7188,8 +7310,12 @@
       <c r="K136" t="s">
         <v>453</v>
       </c>
-      <c r="L136" s="4"/>
-      <c r="M136" s="4"/>
+      <c r="L136" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M136" s="4" t="s">
+        <v>476</v>
+      </c>
     </row>
     <row r="137" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A137" t="s">
@@ -7222,8 +7348,12 @@
       <c r="K137" t="s">
         <v>453</v>
       </c>
-      <c r="L137" s="4"/>
-      <c r="M137" s="4"/>
+      <c r="L137" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M137" s="4" t="s">
+        <v>476</v>
+      </c>
     </row>
     <row r="138" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A138" t="s">
@@ -7257,7 +7387,7 @@
         <v>451</v>
       </c>
       <c r="L138" s="2">
-        <v>43435</v>
+        <v>43465</v>
       </c>
       <c r="M138" t="s">
         <v>469</v>
@@ -7295,7 +7425,7 @@
         <v>451</v>
       </c>
       <c r="L139" s="2">
-        <v>43435</v>
+        <v>43465</v>
       </c>
       <c r="M139" t="s">
         <v>469</v>
@@ -7371,7 +7501,7 @@
         <v>451</v>
       </c>
       <c r="L141" s="2">
-        <v>43435</v>
+        <v>43465</v>
       </c>
       <c r="M141" t="s">
         <v>469</v>
@@ -7409,7 +7539,7 @@
         <v>451</v>
       </c>
       <c r="L142" s="2">
-        <v>43435</v>
+        <v>43465</v>
       </c>
       <c r="M142" t="s">
         <v>469</v>
@@ -7447,7 +7577,7 @@
         <v>451</v>
       </c>
       <c r="L143" s="2">
-        <v>43435</v>
+        <v>43465</v>
       </c>
       <c r="M143" t="s">
         <v>469</v>
@@ -7485,7 +7615,7 @@
         <v>451</v>
       </c>
       <c r="L144" s="2">
-        <v>43435</v>
+        <v>43465</v>
       </c>
       <c r="M144" t="s">
         <v>469</v>
@@ -7523,7 +7653,7 @@
         <v>451</v>
       </c>
       <c r="L145" s="2">
-        <v>43435</v>
+        <v>43465</v>
       </c>
       <c r="M145" t="s">
         <v>469</v>
@@ -7599,7 +7729,7 @@
         <v>451</v>
       </c>
       <c r="L147" s="2">
-        <v>43435</v>
+        <v>43465</v>
       </c>
       <c r="M147" t="s">
         <v>469</v>
@@ -7637,7 +7767,7 @@
         <v>451</v>
       </c>
       <c r="L148" s="2">
-        <v>43435</v>
+        <v>43465</v>
       </c>
       <c r="M148" t="s">
         <v>469</v>
@@ -8869,13 +8999,17 @@
         <v>437</v>
       </c>
       <c r="J182">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="K182" t="s">
         <v>451</v>
       </c>
-      <c r="L182" s="4"/>
-      <c r="M182" s="4"/>
+      <c r="L182" s="2">
+        <v>43312</v>
+      </c>
+      <c r="M182" s="4" t="s">
+        <v>475</v>
+      </c>
     </row>
     <row r="183" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A183" t="s">
@@ -8903,13 +9037,17 @@
         <v>435</v>
       </c>
       <c r="J183">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="K183" t="s">
         <v>451</v>
       </c>
-      <c r="L183" s="4"/>
-      <c r="M183" s="4"/>
+      <c r="L183" s="2">
+        <v>43312</v>
+      </c>
+      <c r="M183" s="4" t="s">
+        <v>475</v>
+      </c>
     </row>
     <row r="184" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A184" t="s">
@@ -9018,8 +9156,12 @@
       <c r="K186" t="s">
         <v>451</v>
       </c>
-      <c r="L186" s="4"/>
-      <c r="M186" s="4"/>
+      <c r="L186" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M186" s="4" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="187" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A187" t="s">
@@ -9052,8 +9194,12 @@
       <c r="K187" t="s">
         <v>451</v>
       </c>
-      <c r="L187" s="4"/>
-      <c r="M187" s="4"/>
+      <c r="L187" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M187" s="4" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="188" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A188" t="s">
@@ -10217,7 +10363,12 @@
       <c r="K218" t="s">
         <v>451</v>
       </c>
-      <c r="L218" s="4"/>
+      <c r="L218" s="5">
+        <v>43312</v>
+      </c>
+      <c r="M218" t="s">
+        <v>475</v>
+      </c>
     </row>
     <row r="219" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A219" t="s">
@@ -10355,8 +10506,12 @@
       <c r="K222" s="4" t="s">
         <v>453</v>
       </c>
-      <c r="L222" s="4"/>
-      <c r="M222" s="4"/>
+      <c r="L222" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M222" s="4" t="s">
+        <v>476</v>
+      </c>
     </row>
     <row r="223" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A223" t="s">
@@ -10383,10 +10538,18 @@
       <c r="I223" t="s">
         <v>434</v>
       </c>
-      <c r="J223" s="4"/>
-      <c r="K223" s="4"/>
-      <c r="L223" s="4"/>
-      <c r="M223" s="4"/>
+      <c r="J223" s="4">
+        <v>10</v>
+      </c>
+      <c r="K223" s="4" t="s">
+        <v>453</v>
+      </c>
+      <c r="L223" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M223" s="4" t="s">
+        <v>476</v>
+      </c>
     </row>
     <row r="224" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A224" t="s">
@@ -10413,10 +10576,18 @@
       <c r="I224" t="s">
         <v>434</v>
       </c>
-      <c r="J224" s="4"/>
-      <c r="K224" s="4"/>
-      <c r="L224" s="4"/>
-      <c r="M224" s="4"/>
+      <c r="J224" s="4">
+        <v>10</v>
+      </c>
+      <c r="K224" s="4" t="s">
+        <v>453</v>
+      </c>
+      <c r="L224" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M224" s="4" t="s">
+        <v>476</v>
+      </c>
     </row>
     <row r="225" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A225" t="s">
@@ -10443,10 +10614,18 @@
       <c r="I225" t="s">
         <v>434</v>
       </c>
-      <c r="J225" s="4"/>
-      <c r="K225" s="4"/>
-      <c r="L225" s="4"/>
-      <c r="M225" s="4"/>
+      <c r="J225" s="4">
+        <v>10</v>
+      </c>
+      <c r="K225" s="4" t="s">
+        <v>453</v>
+      </c>
+      <c r="L225" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M225" s="4" t="s">
+        <v>476</v>
+      </c>
     </row>
     <row r="226" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A226" t="s">
@@ -10473,10 +10652,18 @@
       <c r="I226" t="s">
         <v>434</v>
       </c>
-      <c r="J226" s="4"/>
-      <c r="K226" s="4"/>
-      <c r="L226" s="4"/>
-      <c r="M226" s="4"/>
+      <c r="J226" s="4">
+        <v>10</v>
+      </c>
+      <c r="K226" s="4" t="s">
+        <v>453</v>
+      </c>
+      <c r="L226" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M226" s="4" t="s">
+        <v>476</v>
+      </c>
     </row>
     <row r="227" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A227" t="s">
@@ -10503,10 +10690,18 @@
       <c r="I227" t="s">
         <v>434</v>
       </c>
-      <c r="J227" s="4"/>
-      <c r="K227" s="4"/>
-      <c r="L227" s="4"/>
-      <c r="M227" s="4"/>
+      <c r="J227" s="4">
+        <v>10</v>
+      </c>
+      <c r="K227" s="4" t="s">
+        <v>453</v>
+      </c>
+      <c r="L227" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M227" s="4" t="s">
+        <v>476</v>
+      </c>
     </row>
     <row r="228" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A228" t="s">
@@ -10533,10 +10728,18 @@
       <c r="I228" t="s">
         <v>435</v>
       </c>
-      <c r="J228" s="4"/>
-      <c r="K228" s="4"/>
-      <c r="L228" s="4"/>
-      <c r="M228" s="4"/>
+      <c r="J228" s="4">
+        <v>10</v>
+      </c>
+      <c r="K228" s="4" t="s">
+        <v>453</v>
+      </c>
+      <c r="L228" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M228" s="4" t="s">
+        <v>476</v>
+      </c>
     </row>
     <row r="229" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A229" t="s">
@@ -10563,10 +10766,18 @@
       <c r="I229" t="s">
         <v>435</v>
       </c>
-      <c r="J229" s="4"/>
-      <c r="K229" s="4"/>
-      <c r="L229" s="4"/>
-      <c r="M229" s="4"/>
+      <c r="J229" s="4">
+        <v>10</v>
+      </c>
+      <c r="K229" s="4" t="s">
+        <v>453</v>
+      </c>
+      <c r="L229" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M229" s="4" t="s">
+        <v>476</v>
+      </c>
     </row>
     <row r="230" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A230" t="s">
@@ -10593,10 +10804,18 @@
       <c r="I230" t="s">
         <v>435</v>
       </c>
-      <c r="J230" s="4"/>
-      <c r="K230" s="4"/>
-      <c r="L230" s="4"/>
-      <c r="M230" s="4"/>
+      <c r="J230" s="4">
+        <v>10</v>
+      </c>
+      <c r="K230" s="4" t="s">
+        <v>453</v>
+      </c>
+      <c r="L230" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M230" s="4" t="s">
+        <v>476</v>
+      </c>
     </row>
     <row r="231" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A231" t="s">
@@ -10623,10 +10842,18 @@
       <c r="I231" t="s">
         <v>435</v>
       </c>
-      <c r="J231" s="4"/>
-      <c r="K231" s="4"/>
-      <c r="L231" s="4"/>
-      <c r="M231" s="4"/>
+      <c r="J231" s="4">
+        <v>10</v>
+      </c>
+      <c r="K231" s="4" t="s">
+        <v>453</v>
+      </c>
+      <c r="L231" s="2">
+        <v>43343</v>
+      </c>
+      <c r="M231" s="4" t="s">
+        <v>476</v>
+      </c>
     </row>
     <row r="232" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A232" t="s">
@@ -10774,7 +11001,7 @@
         <v>451</v>
       </c>
       <c r="L235" s="2">
-        <v>43435</v>
+        <v>43465</v>
       </c>
       <c r="M235" t="s">
         <v>469</v>
@@ -10812,7 +11039,7 @@
         <v>451</v>
       </c>
       <c r="L236" s="2">
-        <v>43435</v>
+        <v>43465</v>
       </c>
       <c r="M236" t="s">
         <v>469</v>
@@ -10850,7 +11077,7 @@
         <v>451</v>
       </c>
       <c r="L237" s="2">
-        <v>43435</v>
+        <v>43465</v>
       </c>
       <c r="M237" t="s">
         <v>469</v>
@@ -10888,7 +11115,7 @@
         <v>451</v>
       </c>
       <c r="L238" s="2">
-        <v>43435</v>
+        <v>43465</v>
       </c>
       <c r="M238" t="s">
         <v>469</v>
@@ -10926,7 +11153,7 @@
         <v>451</v>
       </c>
       <c r="L239" s="2">
-        <v>43435</v>
+        <v>43465</v>
       </c>
       <c r="M239" t="s">
         <v>469</v>
@@ -10964,7 +11191,7 @@
         <v>451</v>
       </c>
       <c r="L240" s="2">
-        <v>43435</v>
+        <v>43465</v>
       </c>
       <c r="M240" t="s">
         <v>469</v>
@@ -11002,7 +11229,7 @@
         <v>451</v>
       </c>
       <c r="L241" s="2">
-        <v>43435</v>
+        <v>43465</v>
       </c>
       <c r="M241" t="s">
         <v>469</v>
@@ -11040,7 +11267,7 @@
         <v>451</v>
       </c>
       <c r="L242" s="2">
-        <v>43435</v>
+        <v>43465</v>
       </c>
       <c r="M242" t="s">
         <v>469</v>
@@ -11078,7 +11305,7 @@
         <v>451</v>
       </c>
       <c r="L243" s="2">
-        <v>43435</v>
+        <v>43465</v>
       </c>
       <c r="M243" t="s">
         <v>469</v>
@@ -11116,7 +11343,7 @@
         <v>451</v>
       </c>
       <c r="L244" s="2">
-        <v>43435</v>
+        <v>43465</v>
       </c>
       <c r="M244" t="s">
         <v>469</v>
@@ -11153,8 +11380,12 @@
       <c r="K245" t="s">
         <v>451</v>
       </c>
-      <c r="L245" s="4"/>
-      <c r="M245" s="4"/>
+      <c r="L245" s="5">
+        <v>43343</v>
+      </c>
+      <c r="M245" s="4" t="s">
+        <v>474</v>
+      </c>
     </row>
     <row r="246" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A246" t="s">
@@ -11187,8 +11418,12 @@
       <c r="K246" t="s">
         <v>451</v>
       </c>
-      <c r="L246" s="4"/>
-      <c r="M246" s="4"/>
+      <c r="L246" s="5">
+        <v>43343</v>
+      </c>
+      <c r="M246" s="4" t="s">
+        <v>474</v>
+      </c>
     </row>
     <row r="247" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A247" t="s">
@@ -11221,8 +11456,12 @@
       <c r="K247" t="s">
         <v>451</v>
       </c>
-      <c r="L247" s="4"/>
-      <c r="M247" s="4"/>
+      <c r="L247" s="5">
+        <v>43343</v>
+      </c>
+      <c r="M247" s="4" t="s">
+        <v>474</v>
+      </c>
     </row>
     <row r="248" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A248" t="s">
@@ -11255,8 +11494,12 @@
       <c r="K248" t="s">
         <v>451</v>
       </c>
-      <c r="L248" s="4"/>
-      <c r="M248" s="4"/>
+      <c r="L248" s="5">
+        <v>43343</v>
+      </c>
+      <c r="M248" s="4" t="s">
+        <v>474</v>
+      </c>
     </row>
     <row r="249" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A249" t="s">
@@ -11689,7 +11932,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
fixed latency problems and started graphing code
</commit_message>
<xml_diff>
--- a/Latency.xlsx
+++ b/Latency.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kthibault/Documents/GitHub/sandbox/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{78E8122F-1D0A-FC46-AA1F-952C9AEC7C21}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:8100000_{8A37DFAA-5E58-6B4F-BA52-E6C71243B78F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1240" yWindow="2060" windowWidth="28660" windowHeight="17860" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2235" uniqueCount="478">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2234" uniqueCount="479">
   <si>
     <t>Team</t>
   </si>
@@ -1458,6 +1458,9 @@
   </si>
   <si>
     <t>EcoCore not returning data on time; samples backlogged</t>
+  </si>
+  <si>
+    <t>NEON.DOM.SITE.DP1.20282.001</t>
   </si>
 </sst>
 </file>
@@ -2318,7 +2321,7 @@
       <pane xSplit="4" ySplit="1" topLeftCell="I2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I12" sqref="I12"/>
+      <selection pane="bottomRight" activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2535,8 +2538,8 @@
       <c r="I6" t="s">
         <v>435</v>
       </c>
-      <c r="J6" t="s">
-        <v>7</v>
+      <c r="J6">
+        <v>100</v>
       </c>
       <c r="K6" t="s">
         <v>7</v>
@@ -2574,10 +2577,13 @@
         <v>90</v>
       </c>
       <c r="K7" t="s">
-        <v>7</v>
-      </c>
-      <c r="L7" t="s">
-        <v>7</v>
+        <v>453</v>
+      </c>
+      <c r="L7" s="2">
+        <v>43312</v>
+      </c>
+      <c r="M7" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.2">
@@ -2609,10 +2615,13 @@
         <v>90</v>
       </c>
       <c r="K8" t="s">
-        <v>7</v>
-      </c>
-      <c r="L8" t="s">
-        <v>7</v>
+        <v>453</v>
+      </c>
+      <c r="L8" s="2">
+        <v>43312</v>
+      </c>
+      <c r="M8" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
@@ -2644,10 +2653,13 @@
         <v>90</v>
       </c>
       <c r="K9" t="s">
-        <v>7</v>
-      </c>
-      <c r="L9" t="s">
-        <v>7</v>
+        <v>453</v>
+      </c>
+      <c r="L9" s="2">
+        <v>43312</v>
+      </c>
+      <c r="M9" t="s">
+        <v>454</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
@@ -6779,7 +6791,7 @@
         <v>453</v>
       </c>
       <c r="L122" s="2">
-        <v>43343</v>
+        <v>43312</v>
       </c>
       <c r="M122" t="s">
         <v>467</v>
@@ -6817,7 +6829,7 @@
         <v>453</v>
       </c>
       <c r="L123" s="2">
-        <v>43343</v>
+        <v>43312</v>
       </c>
       <c r="M123" t="s">
         <v>467</v>
@@ -6931,7 +6943,7 @@
         <v>453</v>
       </c>
       <c r="L126" s="2">
-        <v>43343</v>
+        <v>43312</v>
       </c>
       <c r="M126" t="s">
         <v>470</v>
@@ -6969,7 +6981,7 @@
         <v>453</v>
       </c>
       <c r="L127" s="2">
-        <v>43343</v>
+        <v>43312</v>
       </c>
       <c r="M127" t="s">
         <v>470</v>
@@ -7007,7 +7019,7 @@
         <v>453</v>
       </c>
       <c r="L128" s="2">
-        <v>43343</v>
+        <v>43312</v>
       </c>
       <c r="M128" t="s">
         <v>470</v>
@@ -9081,7 +9093,7 @@
         <v>453</v>
       </c>
       <c r="L184" s="2">
-        <v>43343</v>
+        <v>43312</v>
       </c>
       <c r="M184" t="s">
         <v>470</v>
@@ -9119,7 +9131,7 @@
         <v>453</v>
       </c>
       <c r="L185" s="2">
-        <v>43343</v>
+        <v>43312</v>
       </c>
       <c r="M185" t="s">
         <v>470</v>
@@ -11050,7 +11062,7 @@
         <v>209</v>
       </c>
       <c r="B237" t="s">
-        <v>386</v>
+        <v>478</v>
       </c>
       <c r="C237" t="s">
         <v>389</v>
@@ -11088,7 +11100,7 @@
         <v>209</v>
       </c>
       <c r="B238" t="s">
-        <v>386</v>
+        <v>478</v>
       </c>
       <c r="C238" t="s">
         <v>389</v>
@@ -11126,7 +11138,7 @@
         <v>209</v>
       </c>
       <c r="B239" t="s">
-        <v>386</v>
+        <v>478</v>
       </c>
       <c r="C239" t="s">
         <v>389</v>
@@ -11164,7 +11176,7 @@
         <v>209</v>
       </c>
       <c r="B240" t="s">
-        <v>386</v>
+        <v>478</v>
       </c>
       <c r="C240" t="s">
         <v>389</v>
@@ -11202,7 +11214,7 @@
         <v>209</v>
       </c>
       <c r="B241" t="s">
-        <v>386</v>
+        <v>478</v>
       </c>
       <c r="C241" t="s">
         <v>389</v>
@@ -11240,7 +11252,7 @@
         <v>209</v>
       </c>
       <c r="B242" t="s">
-        <v>386</v>
+        <v>478</v>
       </c>
       <c r="C242" t="s">
         <v>389</v>
@@ -11924,6 +11936,7 @@
   </sheetData>
   <autoFilter ref="A1:I260" xr:uid="{F920CE2C-728A-1C45-9F6A-0B2E6D995C2C}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
 

</xml_diff>